<commit_message>
Espruino program to send xy co-ordinates of ultrasonic transducer to node-RED
Simple Espruino program that maintains a rolling average of the last
120ms of ultrasonic sensor readings and then sends them to node-RED as
a set of x,y co-ordinates relative to the centre of the dog based on
the interpretation of a trained neural net.
</commit_message>
<xml_diff>
--- a/espruino/xyanalog.xlsx
+++ b/espruino/xyanalog.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="17400" yWindow="4400" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="xyanalog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -213,604 +213,604 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="447"/>
                 <c:pt idx="0">
-                  <c:v>2.2432182230815</c:v>
+                  <c:v>2.087245837399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.061615244279499</c:v>
+                  <c:v>2.33530439309</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.379165706795</c:v>
+                  <c:v>3.013383250237</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.312262128843999</c:v>
+                  <c:v>3.031205940183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2839890123495</c:v>
+                  <c:v>2.973859883457</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2839757593515</c:v>
+                  <c:v>2.974974429139</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.008051365713</c:v>
+                  <c:v>2.974978970524</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.008053826738</c:v>
+                  <c:v>2.399759649364</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.008293166634</c:v>
+                  <c:v>2.399188391294</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0082950458225</c:v>
+                  <c:v>2.399190615496</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0082973339335</c:v>
+                  <c:v>2.399190608764</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.003702152135</c:v>
+                  <c:v>1.787926095469</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.971085442379</c:v>
+                  <c:v>1.744948163353</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.948946719054</c:v>
+                  <c:v>1.593318317505</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.893289974939</c:v>
+                  <c:v>1.594118141242</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.891389080718</c:v>
+                  <c:v>1.592977089564</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.8330384275005</c:v>
+                  <c:v>1.041123760902</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.120855097427</c:v>
+                  <c:v>1.616348004112</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.08807601908</c:v>
+                  <c:v>1.617397941974</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.028014078837</c:v>
+                  <c:v>1.617399476149</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.028092076442</c:v>
+                  <c:v>1.617404059103</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.314142216484</c:v>
+                  <c:v>2.219478208801</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2731088333035</c:v>
+                  <c:v>2.197222721405</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.3329271436635</c:v>
+                  <c:v>2.304575120603</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.33274412976</c:v>
+                  <c:v>2.192461808636</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.24070685163</c:v>
+                  <c:v>2.189801071872</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5166321756915</c:v>
+                  <c:v>2.624953094099</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.5166318927635</c:v>
+                  <c:v>2.625362190742</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3555849747755</c:v>
+                  <c:v>2.558754096186</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.326309621079</c:v>
+                  <c:v>2.438628681525</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.32630732962</c:v>
+                  <c:v>2.438780093781</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.283013556249</c:v>
+                  <c:v>2.408806224167</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.9989733987205</c:v>
+                  <c:v>2.348994945202</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.0064729853545</c:v>
+                  <c:v>2.361279166724</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.058704795217</c:v>
+                  <c:v>2.473026450884</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.8029425534815</c:v>
+                  <c:v>2.291612631388</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.8312619732225</c:v>
+                  <c:v>2.408311257284</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.83105709803</c:v>
+                  <c:v>2.407901594785</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.8641236627445</c:v>
+                  <c:v>2.152415853365</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.7250731667365</c:v>
+                  <c:v>2.213990560633</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.3874197580255</c:v>
+                  <c:v>2.213834565459</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.268364404105</c:v>
+                  <c:v>2.157220888331</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.9311220890225</c:v>
+                  <c:v>1.648951852239</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.5484667833235</c:v>
+                  <c:v>1.651666803985</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.2408221931025</c:v>
+                  <c:v>1.64438313955</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.00142237961750009</c:v>
+                  <c:v>1.314272475575</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.3624814607935</c:v>
+                  <c:v>1.254212689161</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-0.713671543734</c:v>
+                  <c:v>1.254212601275</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-0.552852556238</c:v>
+                  <c:v>1.575831472124</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.8939071068825</c:v>
+                  <c:v>1.23615577284</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-0.907853276263</c:v>
+                  <c:v>0.561004950592</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-1.166093085355</c:v>
+                  <c:v>0.379507919879</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-0.943081694852</c:v>
+                  <c:v>0.213292325806</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-0.934284682854</c:v>
+                  <c:v>-0.554733237338</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-1.272214143751</c:v>
+                  <c:v>-1.162738753345</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-1.352613993525</c:v>
+                  <c:v>-1.31711723481</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-1.7253323399195</c:v>
+                  <c:v>-1.979175610748</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-2.073353150681501</c:v>
+                  <c:v>-2.681555688743</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-2.3378407520005</c:v>
+                  <c:v>-2.6815365846</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-2.397079316324</c:v>
+                  <c:v>-3.023969986605</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-2.363279806697</c:v>
+                  <c:v>-2.376711503118</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-2.4879822422675</c:v>
+                  <c:v>-2.711694090589</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-2.3783248749305</c:v>
+                  <c:v>-2.09945571551</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-2.1588039783945</c:v>
+                  <c:v>-1.31383612837</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-1.8276943134335</c:v>
+                  <c:v>-1.381689534157</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-1.616657901771</c:v>
+                  <c:v>-1.38811075224</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-1.5124079797195</c:v>
+                  <c:v>-1.471489069091</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-1.334358087407</c:v>
+                  <c:v>-1.46515061262</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-1.334366547242</c:v>
+                  <c:v>-1.994144919401</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-1.3282149933845</c:v>
+                  <c:v>-1.770188646043</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-1.692365353421</c:v>
+                  <c:v>-2.349848110276</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-1.6895954953545</c:v>
+                  <c:v>-2.264270393946</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>-1.977730678779</c:v>
+                  <c:v>-2.657194034351</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-2.2674277305495</c:v>
+                  <c:v>-3.003771828419</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>-2.272336500435</c:v>
+                  <c:v>-2.27369909271</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-2.2772941506985</c:v>
+                  <c:v>-1.845205051302</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-1.885863460056499</c:v>
+                  <c:v>-1.553326890348</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-1.530231472628</c:v>
+                  <c:v>-1.203565562194</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-1.622714285839</c:v>
+                  <c:v>-0.674588175083</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-1.6214577335755</c:v>
+                  <c:v>-0.886241340726</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-1.5747739122895</c:v>
+                  <c:v>-1.034882596566</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-1.314518769139</c:v>
+                  <c:v>-1.114920596763</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-1.314530191117</c:v>
+                  <c:v>-1.298267323207</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-1.141243715262</c:v>
+                  <c:v>-1.53108363268</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-1.427677843965</c:v>
+                  <c:v>-2.27097390816</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>-1.3175848332555</c:v>
+                  <c:v>-2.709383250095</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>-1.060776584221</c:v>
+                  <c:v>-2.218400029764999</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>-0.8478847785585</c:v>
+                  <c:v>-1.856897383062</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>-0.747841118017</c:v>
+                  <c:v>-2.570840396595</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>-0.6407579057185</c:v>
+                  <c:v>-2.356674126425</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>-0.2626598621365</c:v>
+                  <c:v>-2.114665228013</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.0375998411859999</c:v>
+                  <c:v>-1.514116941515</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.3149413973355</c:v>
+                  <c:v>-1.330793059027</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.304795373053</c:v>
+                  <c:v>-0.751403797844</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.722091074586</c:v>
+                  <c:v>-0.58438177977</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.059551800244</c:v>
+                  <c:v>0.074213583584</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.070868421382</c:v>
+                  <c:v>0.096846861323</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.063258739941</c:v>
+                  <c:v>0.161127825945</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.436404447831</c:v>
+                  <c:v>1.075158160561</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.689822037413</c:v>
+                  <c:v>1.075158314988</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.9476219680605</c:v>
+                  <c:v>1.58934550374</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.004835852653</c:v>
+                  <c:v>1.589316623887</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.1656561170485</c:v>
+                  <c:v>1.960675853698</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.294147677973</c:v>
+                  <c:v>1.36099454395</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>2.5053715601625</c:v>
+                  <c:v>2.028563928942</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>2.376339356986</c:v>
+                  <c:v>2.044890016904</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>2.386089925966</c:v>
+                  <c:v>2.044889981441</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>2.238046191538</c:v>
+                  <c:v>1.965389653937</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2.173006934384</c:v>
+                  <c:v>1.797650735101</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>2.4300990145765</c:v>
+                  <c:v>2.304485759838</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.3235043020155</c:v>
+                  <c:v>2.305898432381</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2.533212166851</c:v>
+                  <c:v>2.420355081419</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.5673995227435</c:v>
+                  <c:v>2.370636380399</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>2.867240130010999</c:v>
+                  <c:v>3.227300811996</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>2.8020376184265</c:v>
+                  <c:v>2.982179191383</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>2.814537714725</c:v>
+                  <c:v>2.707788697068</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>2.8510479778215</c:v>
+                  <c:v>2.727289870491</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>2.8531872670055</c:v>
+                  <c:v>2.510702729139</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>2.8370101163145</c:v>
+                  <c:v>2.548363133667</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>2.8644498347525</c:v>
+                  <c:v>2.555712269315</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2.8637449066705</c:v>
+                  <c:v>2.34111017165</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2.8065465104345</c:v>
+                  <c:v>2.646069252283</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>2.9028297482805</c:v>
+                  <c:v>2.764162665088</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2.8190938580105</c:v>
+                  <c:v>2.507179448026</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2.6509953662375</c:v>
+                  <c:v>2.62189604547</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2.803643892126499</c:v>
+                  <c:v>2.921286732382</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>2.9664211646535</c:v>
+                  <c:v>2.974806085152</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>3.0747111059505</c:v>
+                  <c:v>3.195671804872</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>3.0397037529935</c:v>
+                  <c:v>3.125657098962</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>3.080307499611</c:v>
+                  <c:v>3.17318740019</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>3.1869073692695</c:v>
+                  <c:v>3.386379641691</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>2.999850172347501</c:v>
+                  <c:v>2.967023768586</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>3.037086703791</c:v>
+                  <c:v>3.041496831473</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>3.0370875197635</c:v>
+                  <c:v>3.131008267995</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>2.8107657279215</c:v>
+                  <c:v>2.680094687005</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>2.80358917423</c:v>
+                  <c:v>2.686001051871</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>2.7670789085325</c:v>
+                  <c:v>2.958036244155</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>2.799209753433499</c:v>
+                  <c:v>2.953750407028999</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>2.7992105426315</c:v>
+                  <c:v>2.953750407025</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>2.517990963382</c:v>
+                  <c:v>2.987427599032</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>2.4659494044905</c:v>
+                  <c:v>2.987435096848</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>2.465920347623</c:v>
+                  <c:v>3.032676576109</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>2.4659211895095</c:v>
+                  <c:v>3.032676576109</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>2.421166301874</c:v>
+                  <c:v>2.943166771532</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>2.6407940728435</c:v>
+                  <c:v>2.941436768838</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>2.634303141641</c:v>
+                  <c:v>2.921177296589</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>2.5077037881105</c:v>
+                  <c:v>2.57612157291</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>2.5551950252445</c:v>
+                  <c:v>2.644669099838</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>2.6035112560335</c:v>
+                  <c:v>2.644670678238</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>2.6118646453195</c:v>
+                  <c:v>2.048554327732</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>2.661312426093</c:v>
+                  <c:v>1.944463712133</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>2.682703405971</c:v>
+                  <c:v>1.899164119137</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>2.730727988625</c:v>
+                  <c:v>1.89916580291</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>2.764279034322</c:v>
+                  <c:v>1.899165832216</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>3.026946619312501</c:v>
+                  <c:v>2.340151376849</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>3.066828165172</c:v>
+                  <c:v>2.347428986693</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>3.1447176050985</c:v>
+                  <c:v>2.439286003311</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>3.1107039614165</c:v>
+                  <c:v>2.465720950651</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>3.0290257145635</c:v>
+                  <c:v>2.562351833829</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>3.242999180771</c:v>
+                  <c:v>3.175174962907</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>3.1488073022775</c:v>
+                  <c:v>3.378161140053</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>3.158154730327</c:v>
+                  <c:v>3.466242692805</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>3.1040734003095</c:v>
+                  <c:v>3.56229017434</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>3.104073651634</c:v>
+                  <c:v>3.629392236428</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>3.1166831201715</c:v>
+                  <c:v>3.713741861776</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>3.147856531276</c:v>
+                  <c:v>3.786227343651</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>3.11240157969</c:v>
+                  <c:v>3.850149206885999</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>3.0910031805375</c:v>
+                  <c:v>3.755686972182</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>3.078028582616</c:v>
+                  <c:v>3.495699595298</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>3.125957366707</c:v>
+                  <c:v>3.310823398635</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>3.0660930670425</c:v>
+                  <c:v>2.919453464502</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>3.050805169452</c:v>
+                  <c:v>2.850066767849</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>3.002783223886</c:v>
+                  <c:v>2.645856626279</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>3.011134102778</c:v>
+                  <c:v>2.57875506684</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>2.9689582847155</c:v>
+                  <c:v>2.519624378567</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>2.965468741947</c:v>
+                  <c:v>2.509485718901</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>2.887784240366</c:v>
+                  <c:v>2.374653952494</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>2.887524120583</c:v>
+                  <c:v>2.426319388893</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>3.0285647916715</c:v>
+                  <c:v>2.660357569934</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>3.1435065789965</c:v>
+                  <c:v>2.941091334779</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>3.289738074971</c:v>
+                  <c:v>3.212732669583</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>3.375400303217</c:v>
+                  <c:v>3.251543571055</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>3.4536316118745</c:v>
+                  <c:v>3.359709821493</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>3.491789133622001</c:v>
+                  <c:v>3.443513138716001</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>3.610587849377</c:v>
+                  <c:v>3.418292190864</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>3.640520997504</c:v>
+                  <c:v>3.421451764993</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>3.654845031804999</c:v>
+                  <c:v>3.400914528238</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>3.638398219487999</c:v>
+                  <c:v>3.348728852273</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>3.638837732340499</c:v>
+                  <c:v>3.396772013409</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>3.546186713617499</c:v>
+                  <c:v>3.345921823214</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>3.570091970624</c:v>
+                  <c:v>3.366743480359</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>3.5413389821975</c:v>
+                  <c:v>3.499257035379</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>3.325984415496999</c:v>
+                  <c:v>3.547553402256</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>3.317057312476</c:v>
+                  <c:v>3.540065128528</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>3.351890914127</c:v>
+                  <c:v>3.80288350789</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>3.332516081611</c:v>
+                  <c:v>3.859590230015</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>3.2527350772875</c:v>
+                  <c:v>3.908775535372</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>3.2527350772875</c:v>
+                  <c:v>3.928067586703</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>3.2205278463285</c:v>
+                  <c:v>3.880903451272</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>3.1421816817015</c:v>
+                  <c:v>3.746451604021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -822,604 +822,604 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="447"/>
                 <c:pt idx="0">
-                  <c:v>0.2352968036025</c:v>
+                  <c:v>0.162973285369</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.520820593153</c:v>
+                  <c:v>0.753164039182</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.461413220305</c:v>
+                  <c:v>0.291118497104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.609618960937</c:v>
+                  <c:v>0.091715981371</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.693276721109</c:v>
+                  <c:v>0.246801032571</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.693295439441</c:v>
+                  <c:v>0.26537526724</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.827505657226</c:v>
+                  <c:v>0.265437866862</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.827539582089</c:v>
+                  <c:v>0.183090452111</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.883121524991</c:v>
+                  <c:v>0.307589747282</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.883147439452</c:v>
+                  <c:v>0.307620414578</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.8831789795375</c:v>
+                  <c:v>0.307620321836</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.964640185296</c:v>
+                  <c:v>0.288477147124</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.107253324108</c:v>
+                  <c:v>0.631707943506</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2565108533795</c:v>
+                  <c:v>1.127521940503</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.468993249305</c:v>
+                  <c:v>1.139752409647</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.5902979971985</c:v>
+                  <c:v>1.121215611642</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.8000431865085</c:v>
+                  <c:v>1.38957344759</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8483785312365</c:v>
+                  <c:v>1.471988712067</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.9548607178925</c:v>
+                  <c:v>1.4586533027</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1603548486985</c:v>
+                  <c:v>1.458674464326</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.168183436542</c:v>
+                  <c:v>1.458737637239</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.320364896332</c:v>
+                  <c:v>1.640803223468</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4007743643445</c:v>
+                  <c:v>1.58279870471</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.283925397917</c:v>
+                  <c:v>1.385499766256</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.280950224186001</c:v>
+                  <c:v>1.798234088963</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.508875399398001</c:v>
+                  <c:v>2.059380382755001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3746780029055</c:v>
+                  <c:v>2.210512925427</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3746741008595</c:v>
+                  <c:v>2.224768350406</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.5034071434245</c:v>
+                  <c:v>2.451068133085</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.6655001715795</c:v>
+                  <c:v>2.862035233071</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.665468585319</c:v>
+                  <c:v>2.877629235845</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.778325163927</c:v>
+                  <c:v>2.999926569196</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.569703508762</c:v>
+                  <c:v>3.218750023979</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.546681728938</c:v>
+                  <c:v>3.182351029578</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.4209110605715</c:v>
+                  <c:v>2.763666359409</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.210015043576</c:v>
+                  <c:v>2.958370416041</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.177259899398499</c:v>
+                  <c:v>2.538843080383999</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.1701276788665</c:v>
+                  <c:v>2.524579851313</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.0014214392075</c:v>
+                  <c:v>2.555746153764</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.994685612449</c:v>
+                  <c:v>2.468965110088</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.062885223795</c:v>
+                  <c:v>2.453307934793</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.159384115056</c:v>
+                  <c:v>2.556723758658</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.09809479191</c:v>
+                  <c:v>1.920656993545</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.130635741682</c:v>
+                  <c:v>1.911012428298</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.1183993051335</c:v>
+                  <c:v>2.078155761734</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.8808780809355</c:v>
+                  <c:v>1.461659671111</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.9714424470095</c:v>
+                  <c:v>1.815676718413</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.043278999928</c:v>
+                  <c:v>1.81567550642</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.8589710320245</c:v>
+                  <c:v>1.447096724651</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.804775196037</c:v>
+                  <c:v>1.52040611481</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.9326594084785</c:v>
+                  <c:v>1.672462512797</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.69978951818</c:v>
+                  <c:v>1.762044471454</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.066545096697</c:v>
+                  <c:v>2.275532590275</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.955328131498</c:v>
+                  <c:v>2.350259055066</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.8726102757705</c:v>
+                  <c:v>2.158642848533</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.998761982589</c:v>
+                  <c:v>2.30009649076</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.9256228145855</c:v>
+                  <c:v>2.127208175605999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.0703421905035</c:v>
+                  <c:v>2.270882493436</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.945605213768</c:v>
+                  <c:v>2.270845339398</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.6614310905895</c:v>
+                  <c:v>2.089144277264</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.57007443066</c:v>
+                  <c:v>2.19285630416</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.2026082628705</c:v>
+                  <c:v>1.637534564906</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.0210164960965</c:v>
+                  <c:v>1.857557603118999</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.7549164613595</c:v>
+                  <c:v>1.56039720793</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.7546113629365</c:v>
+                  <c:v>1.586577703008</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.9906849607885</c:v>
+                  <c:v>1.697427474418</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.8200246999245</c:v>
+                  <c:v>1.724037453565</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.4318105316265</c:v>
+                  <c:v>1.869801887571</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.4318441740165</c:v>
+                  <c:v>1.620365088138</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.4203496676845</c:v>
+                  <c:v>1.233717903915</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.414723948223</c:v>
+                  <c:v>0.94729255716</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.4399211493655</c:v>
+                  <c:v>0.767681960835</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.295896710951</c:v>
+                  <c:v>0.184475389074</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.25784552132</c:v>
+                  <c:v>-0.050564285211</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.316344996569</c:v>
+                  <c:v>-0.077354977135</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.3257544098165</c:v>
+                  <c:v>0.283942447159</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.2271685468425</c:v>
+                  <c:v>-0.083988053716</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.0631110195290001</c:v>
+                  <c:v>-1.006180824318</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.270666742085</c:v>
+                  <c:v>-0.756676740105</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.27572898984</c:v>
+                  <c:v>-0.393018568546</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.210735376464</c:v>
+                  <c:v>-0.117844660714</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.3470891316365</c:v>
+                  <c:v>0.112160337896</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.3471011631805</c:v>
+                  <c:v>0.407318032828</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.464587459582</c:v>
+                  <c:v>0.566255327851</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.35858393505</c:v>
+                  <c:v>0.710044970273</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>-0.331829284328</c:v>
+                  <c:v>0.367566372474</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>-0.2517460022045</c:v>
+                  <c:v>0.538325147401</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>-0.031447557866</c:v>
+                  <c:v>1.132402863376</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>-0.259812233731</c:v>
+                  <c:v>1.298010224275</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>-0.436579153084</c:v>
+                  <c:v>0.944476548226</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>-0.558817284311</c:v>
+                  <c:v>0.539315413642</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>-0.5376144495195</c:v>
+                  <c:v>0.582017925377</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>-0.387649014626</c:v>
+                  <c:v>0.286884293533</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>-0.3715261107365</c:v>
+                  <c:v>0.362919591313</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>-0.5975599657035</c:v>
+                  <c:v>0.00712289982699998</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>-0.6512847692785</c:v>
+                  <c:v>-1.03122494113</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>-0.6565810565665</c:v>
+                  <c:v>-1.04181715181</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>-0.637222283298</c:v>
+                  <c:v>-1.195297979108</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>-0.762981032593</c:v>
+                  <c:v>-1.817634691737</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>-0.5945058390645</c:v>
+                  <c:v>-1.817634854394</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>-0.514307742702</c:v>
+                  <c:v>-1.656949982264</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>-0.6665845678755</c:v>
+                  <c:v>-1.657246824416</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>-0.6193228720315</c:v>
+                  <c:v>-1.062182322785</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>-0.9270558802335</c:v>
+                  <c:v>-1.105971812786</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>-0.6346490898235</c:v>
+                  <c:v>-1.202242831234</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>-0.33963294205</c:v>
+                  <c:v>-0.271344597427</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>-0.3386766803915</c:v>
+                  <c:v>-0.271344961323</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>-0.4784080638435</c:v>
+                  <c:v>-0.0791465874879999</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>-0.344981485781</c:v>
+                  <c:v>0.291672626551</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>-0.264659411642</c:v>
+                  <c:v>0.628623176265</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>-0.425077077585</c:v>
+                  <c:v>0.62833449686</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>-0.76582298945</c:v>
+                  <c:v>0.324077688665</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>-1.2131173053655</c:v>
+                  <c:v>-0.176463421278</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>-1.191223048614</c:v>
+                  <c:v>-0.748139947681</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>-1.0426461916135</c:v>
+                  <c:v>-0.0670553484130001</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>-1.020264591576</c:v>
+                  <c:v>-0.407921286673</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>-1.119248378009</c:v>
+                  <c:v>-0.40600839946</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>-1.124695331473</c:v>
+                  <c:v>-0.877669540199</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>-1.0817809225605</c:v>
+                  <c:v>-0.981635598113</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>-1.2338547063645</c:v>
+                  <c:v>-1.157941999549</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>-1.233690442755</c:v>
+                  <c:v>-1.47848865203</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>-1.08120677098</c:v>
+                  <c:v>-1.855723667565</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>-1.0481584241815</c:v>
+                  <c:v>-2.249771189453</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>-0.861306884676</c:v>
+                  <c:v>-1.634306149547</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>-1.2820512123515</c:v>
+                  <c:v>-2.018237034814</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>-1.1404460208855</c:v>
+                  <c:v>-1.632607896479</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>-1.4868326801255</c:v>
+                  <c:v>-1.832488356558</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>-1.2510521484475</c:v>
+                  <c:v>-1.371721122747</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>-1.1561547106065</c:v>
+                  <c:v>-1.181926247008</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>-1.266067210891</c:v>
+                  <c:v>-1.30976741318</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>-1.1056693081145</c:v>
+                  <c:v>-0.98889223348</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>-0.825750990977</c:v>
+                  <c:v>-0.306689874395</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>-0.5956788832345</c:v>
+                  <c:v>0.15345434109</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>-0.5956676393625</c:v>
+                  <c:v>-0.088307619805</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>-0.3362024659285</c:v>
+                  <c:v>-0.545865389889</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>-0.3563883379705</c:v>
+                  <c:v>-0.648284145292</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>-0.2574045782135</c:v>
+                  <c:v>-1.141177003693</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>-0.3448993971725</c:v>
+                  <c:v>-1.130383174148</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>-0.3448913022485</c:v>
+                  <c:v>-1.130383174205</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>-0.3619956726755</c:v>
+                  <c:v>-1.222367008602</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>-0.5251468689265</c:v>
+                  <c:v>-1.222446382749</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>-0.525490120432</c:v>
+                  <c:v>-1.344812107559</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>-0.525478519411</c:v>
+                  <c:v>-1.344812107559</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>-0.404586093139</c:v>
+                  <c:v>-1.10302765892</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>-0.160829758569</c:v>
+                  <c:v>-0.126539541968</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>-0.1436137984195</c:v>
+                  <c:v>-0.0644925306489999</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>0.0778934083535</c:v>
+                  <c:v>0.626367847266</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>-0.050059312044</c:v>
+                  <c:v>0.440584379803</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>-0.1801235923155</c:v>
+                  <c:v>0.440600569708</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>-0.201910875763</c:v>
+                  <c:v>0.498375663251</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>-0.33487415243</c:v>
+                  <c:v>0.172152644896</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>-0.393060287892</c:v>
+                  <c:v>0.293831866695</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>-0.522379783716</c:v>
+                  <c:v>0.293855068737</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>-0.613319928865</c:v>
+                  <c:v>0.293855472642</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>-0.9719338622395</c:v>
+                  <c:v>-0.19511997517</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>-1.08456082615</c:v>
+                  <c:v>-0.22273506619</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>-1.276725805811</c:v>
+                  <c:v>-0.470581030559</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>-1.128555690221</c:v>
+                  <c:v>-0.540703003891</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>-0.910616502109</c:v>
+                  <c:v>-0.800847754339</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>-0.6449400685645</c:v>
+                  <c:v>-0.902197414777</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>-0.2021413528415</c:v>
+                  <c:v>-0.841900949756</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>-0.2264449177005</c:v>
+                  <c:v>-1.079952442479</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>-0.4627165935955</c:v>
+                  <c:v>-1.338614636169</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>-0.4627131295535</c:v>
+                  <c:v>-1.520495330372</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>-0.495842925393</c:v>
+                  <c:v>-1.748747749309</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>-0.5810183079015</c:v>
+                  <c:v>-1.94638658611</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>-0.484129497619</c:v>
+                  <c:v>-2.082870581063</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>-0.426576655829</c:v>
+                  <c:v>-1.716408376551</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>-0.3923160544025</c:v>
+                  <c:v>-1.020385249879</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>-0.4918537775795</c:v>
+                  <c:v>-0.387682722352</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>-0.4952553522595</c:v>
+                  <c:v>0.437618244073</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>-0.4539883239115</c:v>
+                  <c:v>0.627062607078</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>-0.3246324747655</c:v>
+                  <c:v>0.413181448978</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>-0.3470987105515</c:v>
+                  <c:v>0.595069071265</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>-0.232986299732</c:v>
+                  <c:v>0.757061898523</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>-0.223625615704</c:v>
+                  <c:v>0.784349970307</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>-0.0319538349295</c:v>
+                  <c:v>1.114611585825</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>-0.0872322167979999</c:v>
+                  <c:v>0.863255064893</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>-0.4625241355505</c:v>
+                  <c:v>0.235753141074</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>-0.8650183275435</c:v>
+                  <c:v>-0.596024832807</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>-1.144692615833</c:v>
+                  <c:v>-1.428128948592</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>-1.296057471635</c:v>
+                  <c:v>-1.535039254901</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>-1.1221444057535</c:v>
+                  <c:v>-1.062446398509</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>-1.1855166643455</c:v>
+                  <c:v>-1.289266492368</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>-1.3997390985605</c:v>
+                  <c:v>-1.223034497987</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>-1.4489820676225</c:v>
+                  <c:v>-1.231601201715</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>-1.4887359256435</c:v>
+                  <c:v>-1.178519255684</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>-1.357640010194</c:v>
+                  <c:v>-1.037719498489</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>-1.3164417644225</c:v>
+                  <c:v>-1.160801412175</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>-1.0959829764205</c:v>
+                  <c:v>-1.13401182228</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>-0.9951528955035</c:v>
+                  <c:v>-0.861256283074</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>-0.9173956885965</c:v>
+                  <c:v>-1.057075688369</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>-1.146996856717</c:v>
+                  <c:v>-1.181842412998</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>-1.098907540372</c:v>
+                  <c:v>-1.081766836323</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>-1.1933336534305</c:v>
+                  <c:v>-1.576443699134</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>-1.072610796194</c:v>
+                  <c:v>-1.66636293353</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>-1.235351413362</c:v>
+                  <c:v>-1.798952595603</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>-1.235351413362</c:v>
+                  <c:v>-1.677560521899</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>-1.151328545659001</c:v>
+                  <c:v>-1.47208211667</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>-1.211199533247</c:v>
+                  <c:v>-1.057954130561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2698,11 +2698,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1827951712"/>
-        <c:axId val="1811494224"/>
+        <c:axId val="-2096576272"/>
+        <c:axId val="1789095552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1827951712"/>
+        <c:axId val="-2096576272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2723,13 +2723,15 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2752,12 +2754,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1811494224"/>
+        <c:crossAx val="1789095552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1811494224"/>
+        <c:axId val="1789095552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2812,7 +2814,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1827951712"/>
+        <c:crossAx val="-2096576272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3773,8 +3775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D27" zoomScale="88" workbookViewId="0">
-      <selection activeCell="P65" sqref="P65"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="88" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3793,12 +3795,12 @@
         <v>0.23529680360250005</v>
       </c>
       <c r="H1">
-        <f>AVERAGE(B1:B20)</f>
-        <v>2.2432182230814997</v>
+        <f>AVERAGE(B1:B10)</f>
+        <v>2.0872458373989997</v>
       </c>
       <c r="I1">
-        <f>AVERAGE(C1:C20)</f>
-        <v>0.23529680360250005</v>
+        <f>AVERAGE(C1:C10)</f>
+        <v>0.16297328536900008</v>
       </c>
       <c r="J1">
         <v>3.1715592057830002</v>
@@ -3821,12 +3823,12 @@
         <v>0.520820593153</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:I2" si="0">AVERAGE(B2:B21)</f>
-        <v>2.0616152442794995</v>
+        <f t="shared" ref="H2:I2" si="0">AVERAGE(B2:B11)</f>
+        <v>2.3353043930899999</v>
       </c>
       <c r="I2">
         <f t="shared" si="0"/>
-        <v>0.520820593153</v>
+        <v>0.75316403918200003</v>
       </c>
       <c r="J2">
         <v>3.1347507751819998</v>
@@ -3849,12 +3851,12 @@
         <v>0.46141322030500004</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:I3" si="1">AVERAGE(B3:B22)</f>
-        <v>2.3791657067949998</v>
+        <f t="shared" ref="H3:I3" si="1">AVERAGE(B3:B12)</f>
+        <v>3.0133832502369997</v>
       </c>
       <c r="I3">
         <f t="shared" si="1"/>
-        <v>0.46141322030500004</v>
+        <v>0.29111849710400001</v>
       </c>
       <c r="J3">
         <v>3.1505179416134999</v>
@@ -3877,12 +3879,12 @@
         <v>0.60961896093699997</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:I4" si="2">AVERAGE(B4:B23)</f>
-        <v>2.3122621288439995</v>
+        <f t="shared" ref="H4:I4" si="2">AVERAGE(B4:B13)</f>
+        <v>3.0312059401829998</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>0.60961896093699997</v>
+        <v>9.1715981371000024E-2</v>
       </c>
       <c r="J4">
         <v>2.9315488245395001</v>
@@ -3905,12 +3907,12 @@
         <v>0.69327672110899996</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:I5" si="3">AVERAGE(B5:B24)</f>
-        <v>2.2839890123495001</v>
+        <f t="shared" ref="H5:I5" si="3">AVERAGE(B5:B14)</f>
+        <v>2.973859883457</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>0.69327672110899996</v>
+        <v>0.24680103257100003</v>
       </c>
       <c r="J5">
         <v>2.8280356033179999</v>
@@ -3933,12 +3935,12 @@
         <v>0.69329543944100003</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:I6" si="4">AVERAGE(B6:B25)</f>
-        <v>2.2839757593514998</v>
+        <f t="shared" ref="H6:I6" si="4">AVERAGE(B6:B15)</f>
+        <v>2.9749744291390003</v>
       </c>
       <c r="I6">
         <f t="shared" si="4"/>
-        <v>0.69329543944100003</v>
+        <v>0.26537526723999999</v>
       </c>
       <c r="J6">
         <v>2.4213486839904999</v>
@@ -3961,12 +3963,12 @@
         <v>0.827505657226</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:I7" si="5">AVERAGE(B7:B26)</f>
-        <v>2.0080513657129999</v>
+        <f t="shared" ref="H7:I7" si="5">AVERAGE(B7:B16)</f>
+        <v>2.974978970524</v>
       </c>
       <c r="I7">
         <f t="shared" si="5"/>
-        <v>0.827505657226</v>
+        <v>0.26543786686199999</v>
       </c>
       <c r="J7">
         <v>2.4563771564849999</v>
@@ -3989,12 +3991,12 @@
         <v>0.82753958208900014</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:I8" si="6">AVERAGE(B8:B27)</f>
-        <v>2.0080538267380001</v>
+        <f t="shared" ref="H8:I8" si="6">AVERAGE(B8:B17)</f>
+        <v>2.3997596493639999</v>
       </c>
       <c r="I8">
         <f t="shared" si="6"/>
-        <v>0.82753958208900014</v>
+        <v>0.18309045211100003</v>
       </c>
       <c r="J8">
         <v>2.2366061044170005</v>
@@ -4017,12 +4019,12 @@
         <v>0.88312152499100005</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:I9" si="7">AVERAGE(B9:B28)</f>
-        <v>2.008293166634</v>
+        <f t="shared" ref="H9:I9" si="7">AVERAGE(B9:B18)</f>
+        <v>2.399188391294</v>
       </c>
       <c r="I9">
         <f t="shared" si="7"/>
-        <v>0.88312152499100005</v>
+        <v>0.30758974728200006</v>
       </c>
       <c r="J9">
         <v>2.2454721849904997</v>
@@ -4045,12 +4047,12 @@
         <v>0.88314743945199992</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:I10" si="8">AVERAGE(B10:B29)</f>
-        <v>2.0082950458225</v>
+        <f t="shared" ref="H10:I10" si="8">AVERAGE(B10:B19)</f>
+        <v>2.3991906154960003</v>
       </c>
       <c r="I10">
         <f t="shared" si="8"/>
-        <v>0.88314743945199992</v>
+        <v>0.30762041457799993</v>
       </c>
       <c r="J10">
         <v>2.2626448946785005</v>
@@ -4073,12 +4075,12 @@
         <v>0.88317897953750002</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:I11" si="9">AVERAGE(B11:B30)</f>
-        <v>2.0082973339334997</v>
+        <f t="shared" ref="H11:I11" si="9">AVERAGE(B11:B20)</f>
+        <v>2.3991906087639996</v>
       </c>
       <c r="I11">
         <f t="shared" si="9"/>
-        <v>0.88317897953750002</v>
+        <v>0.30762032183599997</v>
       </c>
       <c r="J11">
         <v>2.2491494853425005</v>
@@ -4101,12 +4103,12 @@
         <v>0.96464018529599982</v>
       </c>
       <c r="H12">
-        <f t="shared" ref="H12:I12" si="10">AVERAGE(B12:B31)</f>
-        <v>2.0037021521349998</v>
+        <f t="shared" ref="H12:I12" si="10">AVERAGE(B12:B21)</f>
+        <v>1.7879260954689997</v>
       </c>
       <c r="I12">
         <f t="shared" si="10"/>
-        <v>0.96464018529599982</v>
+        <v>0.28847714712399997</v>
       </c>
       <c r="J12">
         <v>2.2491512159194995</v>
@@ -4129,12 +4131,12 @@
         <v>1.107253324108</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:I13" si="11">AVERAGE(B13:B32)</f>
-        <v>1.9710854423790001</v>
+        <f t="shared" ref="H13:I13" si="11">AVERAGE(B13:B22)</f>
+        <v>1.744948163353</v>
       </c>
       <c r="I13">
         <f t="shared" si="11"/>
-        <v>1.107253324108</v>
+        <v>0.63170794350600001</v>
       </c>
       <c r="J13">
         <v>2.4880406347599999</v>
@@ -4157,12 +4159,12 @@
         <v>1.2565108533795</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:I14" si="12">AVERAGE(B14:B33)</f>
-        <v>1.9489467190540002</v>
+        <f t="shared" ref="H14:I14" si="12">AVERAGE(B14:B23)</f>
+        <v>1.5933183175049999</v>
       </c>
       <c r="I14">
         <f t="shared" si="12"/>
-        <v>1.2565108533795</v>
+        <v>1.1275219405029999</v>
       </c>
       <c r="J14">
         <v>2.4874823013395</v>
@@ -4185,12 +4187,12 @@
         <v>1.468993249305</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:I15" si="13">AVERAGE(B15:B34)</f>
-        <v>1.8932899749390004</v>
+        <f t="shared" ref="H15:I15" si="13">AVERAGE(B15:B24)</f>
+        <v>1.594118141242</v>
       </c>
       <c r="I15">
         <f t="shared" si="13"/>
-        <v>1.468993249305</v>
+        <v>1.139752409647</v>
       </c>
       <c r="J15">
         <v>2.2683049878865003</v>
@@ -4213,12 +4215,12 @@
         <v>1.5902979971985001</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:I16" si="14">AVERAGE(B16:B35)</f>
-        <v>1.8913890807179996</v>
+        <f t="shared" ref="H16:I16" si="14">AVERAGE(B16:B25)</f>
+        <v>1.5929770895640001</v>
       </c>
       <c r="I16">
         <f t="shared" si="14"/>
-        <v>1.5902979971985001</v>
+        <v>1.121215611642</v>
       </c>
       <c r="J16">
         <v>2.2571700866594999</v>
@@ -4241,12 +4243,12 @@
         <v>1.8000431865085003</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:I17" si="15">AVERAGE(B17:B36)</f>
-        <v>1.8330384275004998</v>
+        <f t="shared" ref="H17:I17" si="15">AVERAGE(B17:B26)</f>
+        <v>1.0411237609020001</v>
       </c>
       <c r="I17">
         <f t="shared" si="15"/>
-        <v>1.8000431865085003</v>
+        <v>1.3895734475899999</v>
       </c>
       <c r="J17">
         <v>2.0894014714734999</v>
@@ -4269,12 +4271,12 @@
         <v>1.8483785312365</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:I18" si="16">AVERAGE(B18:B37)</f>
-        <v>2.120855097427</v>
+        <f t="shared" ref="H18:I18" si="16">AVERAGE(B18:B27)</f>
+        <v>1.616348004112</v>
       </c>
       <c r="I18">
         <f t="shared" si="16"/>
-        <v>1.8483785312365</v>
+        <v>1.4719887120670001</v>
       </c>
       <c r="J18">
         <v>1.870585665039</v>
@@ -4297,12 +4299,12 @@
         <v>1.9548607178924999</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:I19" si="17">AVERAGE(B19:B38)</f>
-        <v>2.0880760190799998</v>
+        <f t="shared" ref="H19:I19" si="17">AVERAGE(B19:B28)</f>
+        <v>1.6173979419740001</v>
       </c>
       <c r="I19">
         <f t="shared" si="17"/>
-        <v>1.9548607178924999</v>
+        <v>1.4586533026999997</v>
       </c>
       <c r="J19">
         <v>1.8470401738134996</v>
@@ -4325,12 +4327,12 @@
         <v>2.1603548486984998</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:I20" si="18">AVERAGE(B20:B39)</f>
-        <v>2.0280140788369998</v>
+        <f t="shared" ref="H20:I20" si="18">AVERAGE(B20:B29)</f>
+        <v>1.617399476149</v>
       </c>
       <c r="I20">
         <f t="shared" si="18"/>
-        <v>2.1603548486984998</v>
+        <v>1.4586744643259997</v>
       </c>
       <c r="J20">
         <v>1.8910059975259998</v>
@@ -4353,12 +4355,12 @@
         <v>2.1681834365419999</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:I21" si="19">AVERAGE(B21:B40)</f>
-        <v>2.0280920764419998</v>
+        <f t="shared" ref="H21:I21" si="19">AVERAGE(B21:B30)</f>
+        <v>1.6174040591029999</v>
       </c>
       <c r="I21">
         <f t="shared" si="19"/>
-        <v>2.1681834365419999</v>
+        <v>1.4587376372389997</v>
       </c>
       <c r="J21">
         <v>1.6656426948305001</v>
@@ -4381,12 +4383,12 @@
         <v>2.3203648963319998</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:I22" si="20">AVERAGE(B22:B41)</f>
-        <v>2.314142216484</v>
+        <f t="shared" ref="H22:I22" si="20">AVERAGE(B22:B31)</f>
+        <v>2.2194782088010001</v>
       </c>
       <c r="I22">
         <f t="shared" si="20"/>
-        <v>2.3203648963319998</v>
+        <v>1.6408032234679997</v>
       </c>
       <c r="J22">
         <v>1.4000295899949999</v>
@@ -4409,12 +4411,12 @@
         <v>2.4007743643445001</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:I23" si="21">AVERAGE(B23:B42)</f>
-        <v>2.2731088333035001</v>
+        <f t="shared" ref="H23:I23" si="21">AVERAGE(B23:B32)</f>
+        <v>2.1972227214050002</v>
       </c>
       <c r="I23">
         <f t="shared" si="21"/>
-        <v>2.4007743643445001</v>
+        <v>1.5827987047099998</v>
       </c>
       <c r="J23">
         <v>1.1702724586345001</v>
@@ -4437,12 +4439,12 @@
         <v>2.2839253979170002</v>
       </c>
       <c r="H24">
-        <f t="shared" ref="H24:I24" si="22">AVERAGE(B24:B43)</f>
-        <v>2.3329271436635</v>
+        <f t="shared" ref="H24:I24" si="22">AVERAGE(B24:B33)</f>
+        <v>2.3045751206029998</v>
       </c>
       <c r="I24">
         <f t="shared" si="22"/>
-        <v>2.2839253979170002</v>
+        <v>1.3854997662560002</v>
       </c>
       <c r="J24">
         <v>1.3885577994895002</v>
@@ -4465,12 +4467,12 @@
         <v>2.2809502241860007</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:I25" si="23">AVERAGE(B25:B44)</f>
-        <v>2.33274412976</v>
+        <f t="shared" ref="H25:I25" si="23">AVERAGE(B25:B34)</f>
+        <v>2.1924618086359997</v>
       </c>
       <c r="I25">
         <f t="shared" si="23"/>
-        <v>2.2809502241860007</v>
+        <v>1.7982340889630002</v>
       </c>
       <c r="J25">
         <v>1.2450200368620001</v>
@@ -4493,12 +4495,12 @@
         <v>2.5088753993980006</v>
       </c>
       <c r="H26">
-        <f t="shared" ref="H26:I26" si="24">AVERAGE(B26:B45)</f>
-        <v>2.2407068516300006</v>
+        <f t="shared" ref="H26:I26" si="24">AVERAGE(B26:B35)</f>
+        <v>2.189801071872</v>
       </c>
       <c r="I26">
         <f t="shared" si="24"/>
-        <v>2.5088753993980006</v>
+        <v>2.0593803827550006</v>
       </c>
       <c r="J26">
         <v>1.3700005762545</v>
@@ -4521,12 +4523,12 @@
         <v>2.3746780029055001</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:I27" si="25">AVERAGE(B27:B46)</f>
-        <v>2.5166321756915004</v>
+        <f t="shared" ref="H27:I27" si="25">AVERAGE(B27:B36)</f>
+        <v>2.6249530940989998</v>
       </c>
       <c r="I27">
         <f t="shared" si="25"/>
-        <v>2.3746780029055001</v>
+        <v>2.210512925427</v>
       </c>
       <c r="J27">
         <v>1.3546433552665</v>
@@ -4549,12 +4551,12 @@
         <v>2.3746741008595</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="H28:I28" si="26">AVERAGE(B28:B47)</f>
-        <v>2.5166318927635003</v>
+        <f t="shared" ref="H28:I28" si="26">AVERAGE(B28:B37)</f>
+        <v>2.6253621907419999</v>
       </c>
       <c r="I28">
         <f t="shared" si="26"/>
-        <v>2.3746741008595</v>
+        <v>2.2247683504059999</v>
       </c>
       <c r="J28">
         <v>1.5840669340905</v>
@@ -4577,12 +4579,12 @@
         <v>2.5034071434245</v>
       </c>
       <c r="H29">
-        <f t="shared" ref="H29:I29" si="27">AVERAGE(B29:B48)</f>
-        <v>2.3555849747755002</v>
+        <f t="shared" ref="H29:I29" si="27">AVERAGE(B29:B38)</f>
+        <v>2.5587540961860005</v>
       </c>
       <c r="I29">
         <f t="shared" si="27"/>
-        <v>2.5034071434245</v>
+        <v>2.4510681330849997</v>
       </c>
       <c r="J29">
         <v>1.3663781948235001</v>
@@ -4605,12 +4607,12 @@
         <v>2.6655001715794997</v>
       </c>
       <c r="H30">
-        <f t="shared" ref="H30:I30" si="28">AVERAGE(B30:B49)</f>
-        <v>2.3263096210790004</v>
+        <f t="shared" ref="H30:I30" si="28">AVERAGE(B30:B39)</f>
+        <v>2.4386286815250005</v>
       </c>
       <c r="I30">
         <f t="shared" si="28"/>
-        <v>2.6655001715794997</v>
+        <v>2.8620352330709999</v>
       </c>
       <c r="J30">
         <v>1.3847398049315001</v>
@@ -4633,12 +4635,12 @@
         <v>2.6654685853190001</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:I31" si="29">AVERAGE(B31:B50)</f>
-        <v>2.3263073296199996</v>
+        <f t="shared" ref="H31:I31" si="29">AVERAGE(B31:B40)</f>
+        <v>2.4387800937810002</v>
       </c>
       <c r="I31">
         <f t="shared" si="29"/>
-        <v>2.6654685853190001</v>
+        <v>2.8776292358449997</v>
       </c>
       <c r="J31">
         <v>1.2019617219350001</v>
@@ -4661,12 +4663,12 @@
         <v>2.7783251639270001</v>
       </c>
       <c r="H32">
-        <f t="shared" ref="H32:I32" si="30">AVERAGE(B32:B51)</f>
-        <v>2.2830135562489997</v>
+        <f t="shared" ref="H32:I32" si="30">AVERAGE(B32:B41)</f>
+        <v>2.4088062241669999</v>
       </c>
       <c r="I32">
         <f t="shared" si="30"/>
-        <v>2.7783251639270001</v>
+        <v>2.999926569196</v>
       </c>
       <c r="J32">
         <v>0.98873483924850003</v>
@@ -4689,12 +4691,12 @@
         <v>2.5697035087620002</v>
       </c>
       <c r="H33">
-        <f t="shared" ref="H33:I33" si="31">AVERAGE(B33:B52)</f>
-        <v>1.9989733987205003</v>
+        <f t="shared" ref="H33:I33" si="31">AVERAGE(B33:B42)</f>
+        <v>2.348994945202</v>
       </c>
       <c r="I33">
         <f t="shared" si="31"/>
-        <v>2.5697035087620002</v>
+        <v>3.2187500239789997</v>
       </c>
       <c r="J33">
         <v>1.0381056032970002</v>
@@ -4717,12 +4719,12 @@
         <v>2.5466817289379997</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:I34" si="32">AVERAGE(B34:B53)</f>
-        <v>2.0064729853545002</v>
+        <f t="shared" ref="H34:I34" si="32">AVERAGE(B34:B43)</f>
+        <v>2.3612791667240001</v>
       </c>
       <c r="I34">
         <f t="shared" si="32"/>
-        <v>2.5466817289379997</v>
+        <v>3.1823510295780002</v>
       </c>
       <c r="J34">
         <v>0.96003466821899985</v>
@@ -4745,12 +4747,12 @@
         <v>2.4209110605714996</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:I35" si="33">AVERAGE(B35:B54)</f>
-        <v>2.0587047952169999</v>
+        <f t="shared" ref="H35:I35" si="33">AVERAGE(B35:B44)</f>
+        <v>2.4730264508839999</v>
       </c>
       <c r="I35">
         <f t="shared" si="33"/>
-        <v>2.4209110605714996</v>
+        <v>2.7636663594090001</v>
       </c>
       <c r="J35">
         <v>0.90293563460499993</v>
@@ -4773,12 +4775,12 @@
         <v>2.2100150435759995</v>
       </c>
       <c r="H36">
-        <f t="shared" ref="H36:I36" si="34">AVERAGE(B36:B55)</f>
-        <v>1.8029425534815</v>
+        <f t="shared" ref="H36:I36" si="34">AVERAGE(B36:B45)</f>
+        <v>2.2916126313879999</v>
       </c>
       <c r="I36">
         <f t="shared" si="34"/>
-        <v>2.2100150435759995</v>
+        <v>2.9583704160409998</v>
       </c>
       <c r="J36">
         <v>0.85932677219949982</v>
@@ -4801,12 +4803,12 @@
         <v>2.1772598993984991</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37:I37" si="35">AVERAGE(B37:B56)</f>
-        <v>1.8312619732225</v>
+        <f t="shared" ref="H37:I37" si="35">AVERAGE(B37:B46)</f>
+        <v>2.4083112572840002</v>
       </c>
       <c r="I37">
         <f t="shared" si="35"/>
-        <v>2.1772598993984991</v>
+        <v>2.5388430803839994</v>
       </c>
       <c r="J37">
         <v>0.88710760663249977</v>
@@ -4829,12 +4831,12 @@
         <v>2.1701276788664994</v>
       </c>
       <c r="H38">
-        <f t="shared" ref="H38:I38" si="36">AVERAGE(B38:B57)</f>
-        <v>1.8310570980300001</v>
+        <f t="shared" ref="H38:I38" si="36">AVERAGE(B38:B47)</f>
+        <v>2.4079015947850002</v>
       </c>
       <c r="I38">
         <f t="shared" si="36"/>
-        <v>2.1701276788664994</v>
+        <v>2.5245798513129998</v>
       </c>
       <c r="J38">
         <v>0.83971582711750004</v>
@@ -4857,12 +4859,12 @@
         <v>2.0014214392074998</v>
       </c>
       <c r="H39">
-        <f t="shared" ref="H39:I39" si="37">AVERAGE(B39:B58)</f>
-        <v>1.8641236627444999</v>
+        <f t="shared" ref="H39:I39" si="37">AVERAGE(B39:B48)</f>
+        <v>2.1524158533650004</v>
       </c>
       <c r="I39">
         <f t="shared" si="37"/>
-        <v>2.0014214392074998</v>
+        <v>2.5557461537640003</v>
       </c>
       <c r="J39">
         <v>0.62485754381249969</v>
@@ -4885,12 +4887,12 @@
         <v>1.9946856124489998</v>
       </c>
       <c r="H40">
-        <f t="shared" ref="H40:I40" si="38">AVERAGE(B40:B59)</f>
-        <v>1.7250731667364998</v>
+        <f t="shared" ref="H40:I40" si="38">AVERAGE(B40:B49)</f>
+        <v>2.2139905606330004</v>
       </c>
       <c r="I40">
         <f t="shared" si="38"/>
-        <v>1.9946856124489998</v>
+        <v>2.4689651100880003</v>
       </c>
       <c r="J40">
         <v>0.42557609748149983</v>
@@ -4913,12 +4915,12 @@
         <v>2.0628852237949999</v>
       </c>
       <c r="H41">
-        <f t="shared" ref="H41:I41" si="39">AVERAGE(B41:B60)</f>
-        <v>1.3874197580254999</v>
+        <f t="shared" ref="H41:I41" si="39">AVERAGE(B41:B50)</f>
+        <v>2.2138345654589999</v>
       </c>
       <c r="I41">
         <f t="shared" si="39"/>
-        <v>2.0628852237949999</v>
+        <v>2.453307934793</v>
       </c>
       <c r="J41">
         <v>0.42439582231799988</v>
@@ -4941,12 +4943,12 @@
         <v>2.1593841150560005</v>
       </c>
       <c r="H42">
-        <f t="shared" ref="H42:I42" si="40">AVERAGE(B42:B61)</f>
-        <v>1.2683644041049997</v>
+        <f t="shared" ref="H42:I42" si="40">AVERAGE(B42:B51)</f>
+        <v>2.1572208883309996</v>
       </c>
       <c r="I42">
         <f t="shared" si="40"/>
-        <v>2.1593841150560005</v>
+        <v>2.5567237586580003</v>
       </c>
       <c r="J42">
         <v>0.29842458402299987</v>
@@ -4969,12 +4971,12 @@
         <v>2.0980947919099999</v>
       </c>
       <c r="H43">
-        <f t="shared" ref="H43:I43" si="41">AVERAGE(B43:B62)</f>
-        <v>0.9311220890224996</v>
+        <f t="shared" ref="H43:I43" si="41">AVERAGE(B43:B52)</f>
+        <v>1.6489518522389996</v>
       </c>
       <c r="I43">
         <f t="shared" si="41"/>
-        <v>2.0980947919099999</v>
+        <v>1.9206569935449997</v>
       </c>
       <c r="J43">
         <v>0.39542928523849985</v>
@@ -4997,12 +4999,12 @@
         <v>2.1306357416820001</v>
       </c>
       <c r="H44">
-        <f t="shared" ref="H44:I44" si="42">AVERAGE(B44:B63)</f>
-        <v>0.54846678332349996</v>
+        <f t="shared" ref="H44:I44" si="42">AVERAGE(B44:B53)</f>
+        <v>1.6516668039850004</v>
       </c>
       <c r="I44">
         <f t="shared" si="42"/>
-        <v>2.1306357416820001</v>
+        <v>1.9110124282979999</v>
       </c>
       <c r="J44">
         <v>0.23291830012049997</v>
@@ -5025,12 +5027,12 @@
         <v>2.1183993051334999</v>
       </c>
       <c r="H45">
-        <f t="shared" ref="H45:I45" si="43">AVERAGE(B45:B64)</f>
-        <v>0.2408221931024998</v>
+        <f t="shared" ref="H45:I45" si="43">AVERAGE(B45:B54)</f>
+        <v>1.6443831395499999</v>
       </c>
       <c r="I45">
         <f t="shared" si="43"/>
-        <v>2.1183993051334999</v>
+        <v>2.0781557617340001</v>
       </c>
       <c r="J45">
         <v>9.3190692423999869E-2</v>
@@ -5053,12 +5055,12 @@
         <v>1.8808780809355004</v>
       </c>
       <c r="H46">
-        <f t="shared" ref="H46:I46" si="44">AVERAGE(B46:B65)</f>
-        <v>-1.4223796175000913E-3</v>
+        <f t="shared" ref="H46:I46" si="44">AVERAGE(B46:B55)</f>
+        <v>1.3142724755750002</v>
       </c>
       <c r="I46">
         <f t="shared" si="44"/>
-        <v>1.8808780809355004</v>
+        <v>1.4616596711110001</v>
       </c>
       <c r="J46">
         <v>9.8186281823499783E-2</v>
@@ -5081,12 +5083,12 @@
         <v>1.9714424470095004</v>
       </c>
       <c r="H47">
-        <f t="shared" ref="H47:I47" si="45">AVERAGE(B47:B66)</f>
-        <v>-0.36248146079349974</v>
+        <f t="shared" ref="H47:I47" si="45">AVERAGE(B47:B56)</f>
+        <v>1.2542126891610004</v>
       </c>
       <c r="I47">
         <f t="shared" si="45"/>
-        <v>1.9714424470095004</v>
+        <v>1.8156767184130005</v>
       </c>
       <c r="J47">
         <v>-8.5429005169500014E-2</v>
@@ -5109,12 +5111,12 @@
         <v>2.0432789999280003</v>
       </c>
       <c r="H48">
-        <f t="shared" ref="H48:I48" si="46">AVERAGE(B48:B67)</f>
-        <v>-0.71367154373399999</v>
+        <f t="shared" ref="H48:I48" si="46">AVERAGE(B48:B57)</f>
+        <v>1.2542126012749999</v>
       </c>
       <c r="I48">
         <f t="shared" si="46"/>
-        <v>2.0432789999280003</v>
+        <v>1.8156755064200003</v>
       </c>
       <c r="J48">
         <v>-0.28241505023999997</v>
@@ -5137,12 +5139,12 @@
         <v>1.8589710320245003</v>
       </c>
       <c r="H49">
-        <f t="shared" ref="H49:I49" si="47">AVERAGE(B49:B68)</f>
-        <v>-0.55285255623799989</v>
+        <f t="shared" ref="H49:I49" si="47">AVERAGE(B49:B58)</f>
+        <v>1.5758314721240001</v>
       </c>
       <c r="I49">
         <f t="shared" si="47"/>
-        <v>1.8589710320245003</v>
+        <v>1.447096724651</v>
       </c>
       <c r="J49">
         <v>-0.29235223030250002</v>
@@ -5165,12 +5167,12 @@
         <v>1.804775196037</v>
       </c>
       <c r="H50">
-        <f t="shared" ref="H50:I50" si="48">AVERAGE(B50:B69)</f>
-        <v>-0.89390710688250008</v>
+        <f t="shared" ref="H50:I50" si="48">AVERAGE(B50:B59)</f>
+        <v>1.2361557728399999</v>
       </c>
       <c r="I50">
         <f t="shared" si="48"/>
-        <v>1.804775196037</v>
+        <v>1.5204061148099997</v>
       </c>
       <c r="J50">
         <v>-0.52380305634399993</v>
@@ -5193,12 +5195,12 @@
         <v>1.9326594084785</v>
       </c>
       <c r="H51">
-        <f t="shared" ref="H51:I51" si="49">AVERAGE(B51:B70)</f>
-        <v>-0.90785327626299994</v>
+        <f t="shared" ref="H51:I51" si="49">AVERAGE(B51:B60)</f>
+        <v>0.56100495059199995</v>
       </c>
       <c r="I51">
         <f t="shared" si="49"/>
-        <v>1.9326594084785</v>
+        <v>1.6724625127970001</v>
       </c>
       <c r="J51">
         <v>-0.638111146495</v>
@@ -5221,12 +5223,12 @@
         <v>1.69978951818</v>
       </c>
       <c r="H52">
-        <f t="shared" ref="H52:I52" si="50">AVERAGE(B52:B71)</f>
-        <v>-1.166093085355</v>
+        <f t="shared" ref="H52:I52" si="50">AVERAGE(B52:B61)</f>
+        <v>0.37950791987900001</v>
       </c>
       <c r="I52">
         <f t="shared" si="50"/>
-        <v>1.69978951818</v>
+        <v>1.762044471454</v>
       </c>
       <c r="J52">
         <v>-0.72218909387200003</v>
@@ -5249,12 +5251,12 @@
         <v>2.0665450966969998</v>
       </c>
       <c r="H53">
-        <f t="shared" ref="H53:I53" si="51">AVERAGE(B53:B72)</f>
-        <v>-0.94308169485200022</v>
+        <f t="shared" ref="H53:I53" si="51">AVERAGE(B53:B62)</f>
+        <v>0.21329232580599983</v>
       </c>
       <c r="I53">
         <f t="shared" si="51"/>
-        <v>2.0665450966969998</v>
+        <v>2.2755325902750001</v>
       </c>
       <c r="J53">
         <v>-1.0525776647125</v>
@@ -5277,12 +5279,12 @@
         <v>1.9553281314979998</v>
       </c>
       <c r="H54">
-        <f t="shared" ref="H54:I54" si="52">AVERAGE(B54:B73)</f>
-        <v>-0.93428468285400024</v>
+        <f t="shared" ref="H54:I54" si="52">AVERAGE(B54:B63)</f>
+        <v>-0.55473323733800028</v>
       </c>
       <c r="I54">
         <f t="shared" si="52"/>
-        <v>1.9553281314979998</v>
+        <v>2.3502590550660001</v>
       </c>
       <c r="J54">
         <v>-1.3080374582305001</v>
@@ -5305,12 +5307,12 @@
         <v>1.8726102757705003</v>
       </c>
       <c r="H55">
-        <f t="shared" ref="H55:I55" si="53">AVERAGE(B55:B74)</f>
-        <v>-1.2722141437510002</v>
+        <f t="shared" ref="H55:I55" si="53">AVERAGE(B55:B64)</f>
+        <v>-1.1627387533450002</v>
       </c>
       <c r="I55">
         <f t="shared" si="53"/>
-        <v>1.8726102757705003</v>
+        <v>2.1586428485329998</v>
       </c>
       <c r="J55">
         <v>-1.3236867930059999</v>
@@ -5333,12 +5335,12 @@
         <v>1.998761982589</v>
       </c>
       <c r="H56">
-        <f t="shared" ref="H56:I56" si="54">AVERAGE(B56:B75)</f>
-        <v>-1.3526139935250001</v>
+        <f t="shared" ref="H56:I56" si="54">AVERAGE(B56:B65)</f>
+        <v>-1.31711723481</v>
       </c>
       <c r="I56">
         <f t="shared" si="54"/>
-        <v>1.998761982589</v>
+        <v>2.3000964907599997</v>
       </c>
       <c r="J56">
         <v>-1.54338643825</v>
@@ -5361,12 +5363,12 @@
         <v>1.9256228145855001</v>
       </c>
       <c r="H57">
-        <f t="shared" ref="H57:I57" si="55">AVERAGE(B57:B76)</f>
-        <v>-1.7253323399195</v>
+        <f t="shared" ref="H57:I57" si="55">AVERAGE(B57:B66)</f>
+        <v>-1.9791756107480001</v>
       </c>
       <c r="I57">
         <f t="shared" si="55"/>
-        <v>1.9256228145855001</v>
+        <v>2.1272081756059995</v>
       </c>
       <c r="J57">
         <v>-1.577894881038</v>
@@ -5389,12 +5391,12 @@
         <v>2.0703421905035002</v>
       </c>
       <c r="H58">
-        <f t="shared" ref="H58:I58" si="56">AVERAGE(B58:B77)</f>
-        <v>-2.0733531506815006</v>
+        <f t="shared" ref="H58:I58" si="56">AVERAGE(B58:B67)</f>
+        <v>-2.6815556887430003</v>
       </c>
       <c r="I58">
         <f t="shared" si="56"/>
-        <v>2.0703421905035002</v>
+        <v>2.2708824934360003</v>
       </c>
       <c r="J58">
         <v>-1.6136189184660001</v>
@@ -5417,12 +5419,12 @@
         <v>1.9456052137679998</v>
       </c>
       <c r="H59">
-        <f t="shared" ref="H59:I59" si="57">AVERAGE(B59:B78)</f>
-        <v>-2.3378407520005005</v>
+        <f t="shared" ref="H59:I59" si="57">AVERAGE(B59:B68)</f>
+        <v>-2.6815365846000003</v>
       </c>
       <c r="I59">
         <f t="shared" si="57"/>
-        <v>1.9456052137679998</v>
+        <v>2.2708453393979999</v>
       </c>
       <c r="J59">
         <v>-1.5766376144265</v>
@@ -5445,12 +5447,12 @@
         <v>1.6614310905895</v>
       </c>
       <c r="H60">
-        <f t="shared" ref="H60:I60" si="58">AVERAGE(B60:B79)</f>
-        <v>-2.3970793163240005</v>
+        <f t="shared" ref="H60:I60" si="58">AVERAGE(B60:B69)</f>
+        <v>-3.023969986605</v>
       </c>
       <c r="I60">
         <f t="shared" si="58"/>
-        <v>1.6614310905895</v>
+        <v>2.0891442772639999</v>
       </c>
       <c r="J60">
         <v>-1.7157830656304998</v>
@@ -5473,12 +5475,12 @@
         <v>1.5700744306599996</v>
       </c>
       <c r="H61">
-        <f t="shared" ref="H61:I61" si="59">AVERAGE(B61:B80)</f>
-        <v>-2.3632798066970002</v>
+        <f t="shared" ref="H61:I61" si="59">AVERAGE(B61:B70)</f>
+        <v>-2.3767115031179999</v>
       </c>
       <c r="I61">
         <f t="shared" si="59"/>
-        <v>1.5700744306599996</v>
+        <v>2.1928563041599998</v>
       </c>
       <c r="J61">
         <v>-1.7594244963734997</v>
@@ -5501,12 +5503,12 @@
         <v>1.2026082628705002</v>
       </c>
       <c r="H62">
-        <f t="shared" ref="H62:I62" si="60">AVERAGE(B62:B81)</f>
-        <v>-2.4879822422675004</v>
+        <f t="shared" ref="H62:I62" si="60">AVERAGE(B62:B71)</f>
+        <v>-2.7116940905889999</v>
       </c>
       <c r="I62">
         <f t="shared" si="60"/>
-        <v>1.2026082628705002</v>
+        <v>1.6375345649060002</v>
       </c>
       <c r="J62">
         <v>-1.6790471871520001</v>
@@ -5529,12 +5531,12 @@
         <v>1.0210164960964998</v>
       </c>
       <c r="H63">
-        <f t="shared" ref="H63:I63" si="61">AVERAGE(B63:B82)</f>
-        <v>-2.3783248749304997</v>
+        <f t="shared" ref="H63:I63" si="61">AVERAGE(B63:B72)</f>
+        <v>-2.09945571551</v>
       </c>
       <c r="I63">
         <f t="shared" si="61"/>
-        <v>1.0210164960964998</v>
+        <v>1.8575576031189995</v>
       </c>
       <c r="J63">
         <v>-1.8173718859219996</v>
@@ -5557,12 +5559,12 @@
         <v>0.75491646135949997</v>
       </c>
       <c r="H64">
-        <f t="shared" ref="H64:I64" si="62">AVERAGE(B64:B83)</f>
-        <v>-2.1588039783944999</v>
+        <f t="shared" ref="H64:I64" si="62">AVERAGE(B64:B73)</f>
+        <v>-1.31383612837</v>
       </c>
       <c r="I64">
         <f t="shared" si="62"/>
-        <v>0.75491646135949997</v>
+        <v>1.5603972079299999</v>
       </c>
       <c r="J64">
         <v>-2.0412560403764997</v>
@@ -5585,12 +5587,12 @@
         <v>0.75461136293649966</v>
       </c>
       <c r="H65">
-        <f t="shared" ref="H65:I65" si="63">AVERAGE(B65:B84)</f>
-        <v>-1.8276943134335002</v>
+        <f t="shared" ref="H65:I65" si="63">AVERAGE(B65:B74)</f>
+        <v>-1.3816895341570004</v>
       </c>
       <c r="I65">
         <f t="shared" si="63"/>
-        <v>0.75461136293649966</v>
+        <v>1.5865777030079997</v>
       </c>
       <c r="J65">
         <v>-2.1130452284804999</v>
@@ -5613,12 +5615,12 @@
         <v>0.99068496078849988</v>
       </c>
       <c r="H66">
-        <f t="shared" ref="H66:I66" si="64">AVERAGE(B66:B85)</f>
-        <v>-1.6166579017710003</v>
+        <f t="shared" ref="H66:I66" si="64">AVERAGE(B66:B75)</f>
+        <v>-1.38811075224</v>
       </c>
       <c r="I66">
         <f t="shared" si="64"/>
-        <v>0.99068496078849988</v>
+        <v>1.6974274744179998</v>
       </c>
       <c r="J66">
         <v>-2.0888041645594999</v>
@@ -5641,12 +5643,12 @@
         <v>0.82002469992449956</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:I67" si="65">AVERAGE(B67:B86)</f>
-        <v>-1.5124079797195003</v>
+        <f t="shared" ref="H67:I67" si="65">AVERAGE(B67:B76)</f>
+        <v>-1.4714890690910001</v>
       </c>
       <c r="I67">
         <f t="shared" si="65"/>
-        <v>0.82002469992449956</v>
+        <v>1.7240374535649998</v>
       </c>
       <c r="J67">
         <v>-2.2540796440894999</v>
@@ -5669,12 +5671,12 @@
         <v>0.43181053162649974</v>
       </c>
       <c r="H68">
-        <f t="shared" ref="H68:I68" si="66">AVERAGE(B68:B87)</f>
-        <v>-1.3343580874070002</v>
+        <f t="shared" ref="H68:I68" si="66">AVERAGE(B68:B77)</f>
+        <v>-1.46515061262</v>
       </c>
       <c r="I68">
         <f t="shared" si="66"/>
-        <v>0.43181053162649974</v>
+        <v>1.8698018875709999</v>
       </c>
       <c r="J68">
         <v>-2.3643257939239999</v>
@@ -5697,12 +5699,12 @@
         <v>0.43184417401649994</v>
       </c>
       <c r="H69">
-        <f t="shared" ref="H69:I69" si="67">AVERAGE(B69:B88)</f>
-        <v>-1.3343665472420001</v>
+        <f t="shared" ref="H69:I69" si="67">AVERAGE(B69:B78)</f>
+        <v>-1.9941449194010001</v>
       </c>
       <c r="I69">
         <f t="shared" si="67"/>
-        <v>0.43184417401649994</v>
+        <v>1.6203650881380001</v>
       </c>
       <c r="J69">
         <v>-2.2872943218725004</v>
@@ -5725,12 +5727,12 @@
         <v>0.42034966768449999</v>
       </c>
       <c r="H70">
-        <f t="shared" ref="H70:I70" si="68">AVERAGE(B70:B89)</f>
-        <v>-1.3282149933845</v>
+        <f t="shared" ref="H70:I70" si="68">AVERAGE(B70:B79)</f>
+        <v>-1.7701886460430001</v>
       </c>
       <c r="I70">
         <f t="shared" si="68"/>
-        <v>0.42034966768449999</v>
+        <v>1.2337179039149999</v>
       </c>
       <c r="J70">
         <v>-2.3161059227375</v>
@@ -5753,12 +5755,12 @@
         <v>0.41472394822299991</v>
       </c>
       <c r="H71">
-        <f t="shared" ref="H71:I71" si="69">AVERAGE(B71:B90)</f>
-        <v>-1.6923653534210001</v>
+        <f t="shared" ref="H71:I71" si="69">AVERAGE(B71:B80)</f>
+        <v>-2.3498481102760005</v>
       </c>
       <c r="I71">
         <f t="shared" si="69"/>
-        <v>0.41472394822299991</v>
+        <v>0.94729255715999994</v>
       </c>
       <c r="J71">
         <v>-2.3251002382020003</v>
@@ -5781,12 +5783,12 @@
         <v>0.43992114936549997</v>
       </c>
       <c r="H72">
-        <f t="shared" ref="H72:I72" si="70">AVERAGE(B72:B91)</f>
-        <v>-1.6895954953545</v>
+        <f t="shared" ref="H72:I72" si="70">AVERAGE(B72:B81)</f>
+        <v>-2.264270393946</v>
       </c>
       <c r="I72">
         <f t="shared" si="70"/>
-        <v>0.43992114936549997</v>
+        <v>0.76768196083499995</v>
       </c>
       <c r="J72">
         <v>-2.2848900218380002</v>
@@ -5809,12 +5811,12 @@
         <v>0.29589671095099995</v>
       </c>
       <c r="H73">
-        <f t="shared" ref="H73:I73" si="71">AVERAGE(B73:B92)</f>
-        <v>-1.9777306787789999</v>
+        <f t="shared" ref="H73:I73" si="71">AVERAGE(B73:B82)</f>
+        <v>-2.6571940343509999</v>
       </c>
       <c r="I73">
         <f t="shared" si="71"/>
-        <v>0.29589671095099995</v>
+        <v>0.18447538907399991</v>
       </c>
       <c r="J73">
         <v>-2.3366031968229999</v>
@@ -5837,12 +5839,12 @@
         <v>0.25784552131999994</v>
       </c>
       <c r="H74">
-        <f t="shared" ref="H74:I74" si="72">AVERAGE(B74:B93)</f>
-        <v>-2.2674277305495001</v>
+        <f t="shared" ref="H74:I74" si="72">AVERAGE(B74:B83)</f>
+        <v>-3.003771828419</v>
       </c>
       <c r="I74">
         <f t="shared" si="72"/>
-        <v>0.25784552131999994</v>
+        <v>-5.0564285211000023E-2</v>
       </c>
       <c r="J74">
         <v>-2.3063124075629999</v>
@@ -5865,12 +5867,12 @@
         <v>0.31634499656899995</v>
       </c>
       <c r="H75">
-        <f t="shared" ref="H75:I75" si="73">AVERAGE(B75:B94)</f>
-        <v>-2.2723365004349998</v>
+        <f t="shared" ref="H75:I75" si="73">AVERAGE(B75:B84)</f>
+        <v>-2.2736990927099994</v>
       </c>
       <c r="I75">
         <f t="shared" si="73"/>
-        <v>0.31634499656899995</v>
+        <v>-7.7354977134999989E-2</v>
       </c>
       <c r="J75">
         <v>-2.3599920932164999</v>
@@ -5893,12 +5895,12 @@
         <v>0.3257544098165</v>
       </c>
       <c r="H76">
-        <f t="shared" ref="H76:I76" si="74">AVERAGE(B76:B95)</f>
-        <v>-2.2772941506984994</v>
+        <f t="shared" ref="H76:I76" si="74">AVERAGE(B76:B85)</f>
+        <v>-1.8452050513019997</v>
       </c>
       <c r="I76">
         <f t="shared" si="74"/>
-        <v>0.3257544098165</v>
+        <v>0.28394244715899997</v>
       </c>
       <c r="J76">
         <v>-2.4047765185160004</v>
@@ -5921,12 +5923,12 @@
         <v>0.22716854684249999</v>
       </c>
       <c r="H77">
-        <f t="shared" ref="H77:I77" si="75">AVERAGE(B77:B96)</f>
-        <v>-1.8858634600564994</v>
+        <f t="shared" ref="H77:I77" si="75">AVERAGE(B77:B86)</f>
+        <v>-1.5533268903479995</v>
       </c>
       <c r="I77">
         <f t="shared" si="75"/>
-        <v>0.22716854684249999</v>
+        <v>-8.3988053716000044E-2</v>
       </c>
       <c r="J77">
         <v>-2.4569842528800003</v>
@@ -5949,12 +5951,12 @@
         <v>6.3111019529000084E-2</v>
       </c>
       <c r="H78">
-        <f t="shared" ref="H78:I78" si="76">AVERAGE(B78:B97)</f>
-        <v>-1.530231472628</v>
+        <f t="shared" ref="H78:I78" si="76">AVERAGE(B78:B87)</f>
+        <v>-1.2035655621939998</v>
       </c>
       <c r="I78">
         <f t="shared" si="76"/>
-        <v>6.3111019529000084E-2</v>
+        <v>-1.0061808243179999</v>
       </c>
       <c r="J78">
         <v>-2.4912389963714996</v>
@@ -5977,12 +5979,12 @@
         <v>0.27066674208499991</v>
       </c>
       <c r="H79">
-        <f t="shared" ref="H79:I79" si="77">AVERAGE(B79:B98)</f>
-        <v>-1.622714285839</v>
+        <f t="shared" ref="H79:I79" si="77">AVERAGE(B79:B88)</f>
+        <v>-0.67458817508300006</v>
       </c>
       <c r="I79">
         <f t="shared" si="77"/>
-        <v>0.27066674208499991</v>
+        <v>-0.75667674010500019</v>
       </c>
       <c r="J79">
         <v>-2.6201276198550003</v>
@@ -6005,12 +6007,12 @@
         <v>0.27572898984000005</v>
       </c>
       <c r="H80">
-        <f t="shared" ref="H80:I80" si="78">AVERAGE(B80:B99)</f>
-        <v>-1.6214577335755003</v>
+        <f t="shared" ref="H80:I80" si="78">AVERAGE(B80:B89)</f>
+        <v>-0.88624134072600003</v>
       </c>
       <c r="I80">
         <f t="shared" si="78"/>
-        <v>0.27572898984000005</v>
+        <v>-0.39301856854600004</v>
       </c>
       <c r="J80">
         <v>-2.6348351556354999</v>
@@ -6033,12 +6035,12 @@
         <v>0.21073537646400003</v>
       </c>
       <c r="H81">
-        <f t="shared" ref="H81:I81" si="79">AVERAGE(B81:B100)</f>
-        <v>-1.5747739122894999</v>
+        <f t="shared" ref="H81:I81" si="79">AVERAGE(B81:B90)</f>
+        <v>-1.0348825965660002</v>
       </c>
       <c r="I81">
         <f t="shared" si="79"/>
-        <v>0.21073537646400003</v>
+        <v>-0.11784466071400002</v>
       </c>
       <c r="J81">
         <v>-2.6968535281005002</v>
@@ -6061,12 +6063,12 @@
         <v>0.34708913163650001</v>
       </c>
       <c r="H82">
-        <f t="shared" ref="H82:I82" si="80">AVERAGE(B82:B101)</f>
-        <v>-1.3145187691389997</v>
+        <f t="shared" ref="H82:I82" si="80">AVERAGE(B82:B91)</f>
+        <v>-1.114920596763</v>
       </c>
       <c r="I82">
         <f t="shared" si="80"/>
-        <v>0.34708913163650001</v>
+        <v>0.11216033789599995</v>
       </c>
       <c r="J82">
         <v>-2.7451854615409998</v>
@@ -6089,12 +6091,12 @@
         <v>0.34710116318050011</v>
       </c>
       <c r="H83">
-        <f t="shared" ref="H83:I83" si="81">AVERAGE(B83:B102)</f>
-        <v>-1.3145301911169998</v>
+        <f t="shared" ref="H83:I83" si="81">AVERAGE(B83:B92)</f>
+        <v>-1.2982673232069999</v>
       </c>
       <c r="I83">
         <f t="shared" si="81"/>
-        <v>0.34710116318050011</v>
+        <v>0.40731803282799994</v>
       </c>
       <c r="J83">
         <v>-2.8161924739290001</v>
@@ -6117,12 +6119,12 @@
         <v>0.46458745958199987</v>
       </c>
       <c r="H84">
-        <f t="shared" ref="H84:I84" si="82">AVERAGE(B84:B103)</f>
-        <v>-1.1412437152619996</v>
+        <f t="shared" ref="H84:I84" si="82">AVERAGE(B84:B93)</f>
+        <v>-1.5310836326799999</v>
       </c>
       <c r="I84">
         <f t="shared" si="82"/>
-        <v>0.46458745958199987</v>
+        <v>0.56625532785099997</v>
       </c>
       <c r="J84">
         <v>-2.7686506554429999</v>
@@ -6145,12 +6147,12 @@
         <v>0.35858393504999997</v>
       </c>
       <c r="H85">
-        <f t="shared" ref="H85:I85" si="83">AVERAGE(B85:B104)</f>
-        <v>-1.4276778439649997</v>
+        <f t="shared" ref="H85:I85" si="83">AVERAGE(B85:B94)</f>
+        <v>-2.2709739081599998</v>
       </c>
       <c r="I85">
         <f t="shared" si="83"/>
-        <v>0.35858393504999997</v>
+        <v>0.71004497027299984</v>
       </c>
       <c r="J85">
         <v>-2.7443079007720002</v>
@@ -6173,12 +6175,12 @@
         <v>-0.33182928432799996</v>
       </c>
       <c r="H86">
-        <f t="shared" ref="H86:I86" si="84">AVERAGE(B86:B105)</f>
-        <v>-1.3175848332554998</v>
+        <f t="shared" ref="H86:I86" si="84">AVERAGE(B86:B95)</f>
+        <v>-2.7093832500950001</v>
       </c>
       <c r="I86">
         <f t="shared" si="84"/>
-        <v>-0.33182928432799996</v>
+        <v>0.36756637247399998</v>
       </c>
       <c r="J86">
         <v>-2.8575158399920002</v>
@@ -6201,12 +6203,12 @@
         <v>-0.25174600220450005</v>
       </c>
       <c r="H87">
-        <f t="shared" ref="H87:I87" si="85">AVERAGE(B87:B106)</f>
-        <v>-1.0607765842209997</v>
+        <f t="shared" ref="H87:I87" si="85">AVERAGE(B87:B96)</f>
+        <v>-2.2184000297649993</v>
       </c>
       <c r="I87">
         <f t="shared" si="85"/>
-        <v>-0.25174600220450005</v>
+        <v>0.53832514740100001</v>
       </c>
       <c r="J87">
         <v>-2.8548177864095003</v>
@@ -6229,12 +6231,12 @@
         <v>-3.1447557865999967E-2</v>
       </c>
       <c r="H88">
-        <f t="shared" ref="H88:I88" si="86">AVERAGE(B88:B107)</f>
-        <v>-0.84788477855849975</v>
+        <f t="shared" ref="H88:I88" si="86">AVERAGE(B88:B97)</f>
+        <v>-1.8568973830619999</v>
       </c>
       <c r="I88">
         <f t="shared" si="86"/>
-        <v>-3.1447557865999967E-2</v>
+        <v>1.1324028633759999</v>
       </c>
       <c r="J88">
         <v>-2.8693318077775003</v>
@@ -6257,12 +6259,12 @@
         <v>-0.25981223373099999</v>
       </c>
       <c r="H89">
-        <f t="shared" ref="H89:I89" si="87">AVERAGE(B89:B108)</f>
-        <v>-0.74784111801699971</v>
+        <f t="shared" ref="H89:I89" si="87">AVERAGE(B89:B98)</f>
+        <v>-2.570840396595</v>
       </c>
       <c r="I89">
         <f t="shared" si="87"/>
-        <v>-0.25981223373099999</v>
+        <v>1.2980102242749998</v>
       </c>
       <c r="J89">
         <v>-3.0653516901315001</v>
@@ -6285,12 +6287,12 @@
         <v>-0.43657915308400008</v>
       </c>
       <c r="H90">
-        <f t="shared" ref="H90:I90" si="88">AVERAGE(B90:B109)</f>
-        <v>-0.6407579057185</v>
+        <f t="shared" ref="H90:I90" si="88">AVERAGE(B90:B99)</f>
+        <v>-2.3566741264249997</v>
       </c>
       <c r="I90">
         <f t="shared" si="88"/>
-        <v>-0.43657915308400008</v>
+        <v>0.9444765482259998</v>
       </c>
       <c r="J90">
         <v>-3.1486717709960006</v>
@@ -6313,12 +6315,12 @@
         <v>-0.55881728431099997</v>
       </c>
       <c r="H91">
-        <f t="shared" ref="H91:I91" si="89">AVERAGE(B91:B110)</f>
-        <v>-0.2626598621365</v>
+        <f t="shared" ref="H91:I91" si="89">AVERAGE(B91:B100)</f>
+        <v>-2.1146652280130001</v>
       </c>
       <c r="I91">
         <f t="shared" si="89"/>
-        <v>-0.55881728431099997</v>
+        <v>0.53931541364200009</v>
       </c>
       <c r="J91">
         <v>-3.1559688565415001</v>
@@ -6341,12 +6343,12 @@
         <v>-0.5376144495195001</v>
       </c>
       <c r="H92">
-        <f t="shared" ref="H92:I92" si="90">AVERAGE(B92:B111)</f>
-        <v>3.7599841185999863E-2</v>
+        <f t="shared" ref="H92:I92" si="90">AVERAGE(B92:B101)</f>
+        <v>-1.5141169415150002</v>
       </c>
       <c r="I92">
         <f t="shared" si="90"/>
-        <v>-0.5376144495195001</v>
+        <v>0.58201792537700014</v>
       </c>
       <c r="J92">
         <v>-3.2730555004640003</v>
@@ -6369,12 +6371,12 @@
         <v>-0.38764901462600004</v>
       </c>
       <c r="H93">
-        <f t="shared" ref="H93:I93" si="91">AVERAGE(B93:B112)</f>
-        <v>0.31494139733550003</v>
+        <f t="shared" ref="H93:I93" si="91">AVERAGE(B93:B102)</f>
+        <v>-1.3307930590269998</v>
       </c>
       <c r="I93">
         <f t="shared" si="91"/>
-        <v>-0.38764901462600004</v>
+        <v>0.28688429353299993</v>
       </c>
       <c r="J93">
         <v>-3.2655061982295002</v>
@@ -6397,12 +6399,12 @@
         <v>-0.37152611073650005</v>
       </c>
       <c r="H94">
-        <f t="shared" ref="H94:I94" si="92">AVERAGE(B94:B113)</f>
-        <v>0.30479537305299997</v>
+        <f t="shared" ref="H94:I94" si="92">AVERAGE(B94:B103)</f>
+        <v>-0.75140379784399991</v>
       </c>
       <c r="I94">
         <f t="shared" si="92"/>
-        <v>-0.37152611073650005</v>
+        <v>0.362919591313</v>
       </c>
       <c r="J94">
         <v>-3.2701857373744998</v>
@@ -6425,12 +6427,12 @@
         <v>-0.59755996570350012</v>
       </c>
       <c r="H95">
-        <f t="shared" ref="H95:I95" si="93">AVERAGE(B95:B114)</f>
-        <v>0.72209107458599997</v>
+        <f t="shared" ref="H95:I95" si="93">AVERAGE(B95:B104)</f>
+        <v>-0.58438177976999994</v>
       </c>
       <c r="I95">
         <f t="shared" si="93"/>
-        <v>-0.59755996570350012</v>
+        <v>7.1228998269999844E-3</v>
       </c>
       <c r="J95">
         <v>-3.2518530668479997</v>
@@ -6453,12 +6455,12 @@
         <v>-0.65128476927849999</v>
       </c>
       <c r="H96">
-        <f t="shared" ref="H96:I96" si="94">AVERAGE(B96:B115)</f>
-        <v>1.0595518002439999</v>
+        <f t="shared" ref="H96:I96" si="94">AVERAGE(B96:B105)</f>
+        <v>7.4213583584000015E-2</v>
       </c>
       <c r="I96">
         <f t="shared" si="94"/>
-        <v>-0.65128476927849999</v>
+        <v>-1.0312249411300001</v>
       </c>
       <c r="J96">
         <v>-3.2467433802959995</v>
@@ -6481,12 +6483,12 @@
         <v>-0.65658105656649979</v>
       </c>
       <c r="H97">
-        <f t="shared" ref="H97:I97" si="95">AVERAGE(B97:B116)</f>
-        <v>1.0708684213819999</v>
+        <f t="shared" ref="H97:I97" si="95">AVERAGE(B97:B106)</f>
+        <v>9.684686132299998E-2</v>
       </c>
       <c r="I97">
         <f t="shared" si="95"/>
-        <v>-0.65658105656649979</v>
+        <v>-1.0418171518099999</v>
       </c>
       <c r="J97">
         <v>-3.2601490078834998</v>
@@ -6509,12 +6511,12 @@
         <v>-0.6372222832979999</v>
       </c>
       <c r="H98">
-        <f t="shared" ref="H98:I98" si="96">AVERAGE(B98:B117)</f>
-        <v>1.0632587399409998</v>
+        <f t="shared" ref="H98:I98" si="96">AVERAGE(B98:B107)</f>
+        <v>0.16112782594500002</v>
       </c>
       <c r="I98">
         <f t="shared" si="96"/>
-        <v>-0.6372222832979999</v>
+        <v>-1.1952979791080001</v>
       </c>
       <c r="J98">
         <v>-3.2248613901854997</v>
@@ -6537,12 +6539,12 @@
         <v>-0.76298103259299999</v>
       </c>
       <c r="H99">
-        <f t="shared" ref="H99:I99" si="97">AVERAGE(B99:B118)</f>
-        <v>1.4364044478309999</v>
+        <f t="shared" ref="H99:I99" si="97">AVERAGE(B99:B108)</f>
+        <v>1.0751581605609999</v>
       </c>
       <c r="I99">
         <f t="shared" si="97"/>
-        <v>-0.76298103259299999</v>
+        <v>-1.8176346917370001</v>
       </c>
       <c r="J99">
         <v>-3.2232333730809999</v>
@@ -6565,12 +6567,12 @@
         <v>-0.59450583906450005</v>
       </c>
       <c r="H100">
-        <f t="shared" ref="H100:I100" si="98">AVERAGE(B100:B119)</f>
-        <v>1.6898220374129997</v>
+        <f t="shared" ref="H100:I100" si="98">AVERAGE(B100:B109)</f>
+        <v>1.075158314988</v>
       </c>
       <c r="I100">
         <f t="shared" si="98"/>
-        <v>-0.59450583906450005</v>
+        <v>-1.8176348543940002</v>
       </c>
       <c r="J100">
         <v>-3.2289110283424995</v>
@@ -6593,12 +6595,12 @@
         <v>-0.51430774270199986</v>
       </c>
       <c r="H101">
-        <f t="shared" ref="H101:I101" si="99">AVERAGE(B101:B120)</f>
-        <v>1.9476219680604998</v>
+        <f t="shared" ref="H101:I101" si="99">AVERAGE(B101:B110)</f>
+        <v>1.5893455037399999</v>
       </c>
       <c r="I101">
         <f t="shared" si="99"/>
-        <v>-0.51430774270199986</v>
+        <v>-1.6569499822639997</v>
       </c>
       <c r="J101">
         <v>-3.2252722273309997</v>
@@ -6621,12 +6623,12 @@
         <v>-0.66658456787550002</v>
       </c>
       <c r="H102">
-        <f t="shared" ref="H102:I102" si="100">AVERAGE(B102:B121)</f>
-        <v>2.0048358526529997</v>
+        <f t="shared" ref="H102:I102" si="100">AVERAGE(B102:B111)</f>
+        <v>1.589316623887</v>
       </c>
       <c r="I102">
         <f t="shared" si="100"/>
-        <v>-0.66658456787550002</v>
+        <v>-1.6572468244159999</v>
       </c>
       <c r="J102">
         <v>-3.2301390913175005</v>
@@ -6649,12 +6651,12 @@
         <v>-0.61932287203150005</v>
       </c>
       <c r="H103">
-        <f t="shared" ref="H103:I103" si="101">AVERAGE(B103:B122)</f>
-        <v>2.1656561170485</v>
+        <f t="shared" ref="H103:I103" si="101">AVERAGE(B103:B112)</f>
+        <v>1.960675853698</v>
       </c>
       <c r="I103">
         <f t="shared" si="101"/>
-        <v>-0.61932287203150005</v>
+        <v>-1.062182322785</v>
       </c>
       <c r="J103">
         <v>-3.2365629415525001</v>
@@ -6677,12 +6679,12 @@
         <v>-0.92705588023349994</v>
       </c>
       <c r="H104">
-        <f t="shared" ref="H104:I104" si="102">AVERAGE(B104:B123)</f>
-        <v>2.2941476779730001</v>
+        <f t="shared" ref="H104:I104" si="102">AVERAGE(B104:B113)</f>
+        <v>1.36099454395</v>
       </c>
       <c r="I104">
         <f t="shared" si="102"/>
-        <v>-0.92705588023349994</v>
+        <v>-1.1059718127859999</v>
       </c>
       <c r="J104">
         <v>-3.2160544031699998</v>
@@ -6705,12 +6707,12 @@
         <v>-0.63464908982349999</v>
       </c>
       <c r="H105">
-        <f t="shared" ref="H105:I105" si="103">AVERAGE(B105:B124)</f>
-        <v>2.5053715601624997</v>
+        <f t="shared" ref="H105:I105" si="103">AVERAGE(B105:B114)</f>
+        <v>2.0285639289419999</v>
       </c>
       <c r="I105">
         <f t="shared" si="103"/>
-        <v>-0.63464908982349999</v>
+        <v>-1.2022428312340001</v>
       </c>
       <c r="J105">
         <v>-2.9242959310200005</v>
@@ -6733,12 +6735,12 @@
         <v>-0.33963294205</v>
       </c>
       <c r="H106">
-        <f t="shared" ref="H106:I106" si="104">AVERAGE(B106:B125)</f>
-        <v>2.3763393569860001</v>
+        <f t="shared" ref="H106:I106" si="104">AVERAGE(B106:B115)</f>
+        <v>2.0448900169040001</v>
       </c>
       <c r="I106">
         <f t="shared" si="104"/>
-        <v>-0.33963294205</v>
+        <v>-0.27134459742699996</v>
       </c>
       <c r="J106">
         <v>-2.9303600477635001</v>
@@ -6761,12 +6763,12 @@
         <v>-0.33867668039149995</v>
       </c>
       <c r="H107">
-        <f t="shared" ref="H107:I107" si="105">AVERAGE(B107:B126)</f>
-        <v>2.386089925966</v>
+        <f t="shared" ref="H107:I107" si="105">AVERAGE(B107:B116)</f>
+        <v>2.044889981441</v>
       </c>
       <c r="I107">
         <f t="shared" si="105"/>
-        <v>-0.33867668039149995</v>
+        <v>-0.27134496132299996</v>
       </c>
       <c r="J107">
         <v>-2.7658132645634996</v>
@@ -6789,12 +6791,12 @@
         <v>-0.47840806384349993</v>
       </c>
       <c r="H108">
-        <f t="shared" ref="H108:I108" si="106">AVERAGE(B108:B127)</f>
-        <v>2.2380461915379999</v>
+        <f t="shared" ref="H108:I108" si="106">AVERAGE(B108:B117)</f>
+        <v>1.9653896539369999</v>
       </c>
       <c r="I108">
         <f t="shared" si="106"/>
-        <v>-0.47840806384349993</v>
+        <v>-7.9146587487999936E-2</v>
       </c>
       <c r="J108">
         <v>-2.7714320528415</v>
@@ -6817,12 +6819,12 @@
         <v>-0.34498148578099996</v>
       </c>
       <c r="H109">
-        <f t="shared" ref="H109:I109" si="107">AVERAGE(B109:B128)</f>
-        <v>2.1730069343839999</v>
+        <f t="shared" ref="H109:I109" si="107">AVERAGE(B109:B118)</f>
+        <v>1.797650735101</v>
       </c>
       <c r="I109">
         <f t="shared" si="107"/>
-        <v>-0.34498148578099996</v>
+        <v>0.29167262655100001</v>
       </c>
       <c r="J109">
         <v>-2.7662993346689997</v>
@@ -6845,12 +6847,12 @@
         <v>-0.26465941164200008</v>
       </c>
       <c r="H110">
-        <f t="shared" ref="H110:I110" si="108">AVERAGE(B110:B129)</f>
-        <v>2.4300990145764998</v>
+        <f t="shared" ref="H110:I110" si="108">AVERAGE(B110:B119)</f>
+        <v>2.3044857598379997</v>
       </c>
       <c r="I110">
         <f t="shared" si="108"/>
-        <v>-0.26465941164200008</v>
+        <v>0.62862317626499986</v>
       </c>
       <c r="J110">
         <v>-2.7630137738924998</v>
@@ -6873,12 +6875,12 @@
         <v>-0.42507707758499996</v>
       </c>
       <c r="H111">
-        <f t="shared" ref="H111:I111" si="109">AVERAGE(B111:B130)</f>
-        <v>2.3235043020154995</v>
+        <f t="shared" ref="H111:I111" si="109">AVERAGE(B111:B120)</f>
+        <v>2.3058984323809999</v>
       </c>
       <c r="I111">
         <f t="shared" si="109"/>
-        <v>-0.42507707758499996</v>
+        <v>0.62833449686000009</v>
       </c>
       <c r="J111">
         <v>-2.5911556420174993</v>
@@ -6901,12 +6903,12 @@
         <v>-0.76582298944999994</v>
       </c>
       <c r="H112">
-        <f t="shared" ref="H112:I112" si="110">AVERAGE(B112:B131)</f>
-        <v>2.5332121668509999</v>
+        <f t="shared" ref="H112:I112" si="110">AVERAGE(B112:B121)</f>
+        <v>2.4203550814190002</v>
       </c>
       <c r="I112">
         <f t="shared" si="110"/>
-        <v>-0.76582298944999994</v>
+        <v>0.32407768866500003</v>
       </c>
       <c r="J112">
         <v>-2.3199501226084993</v>
@@ -6929,12 +6931,12 @@
         <v>-1.2131173053655</v>
       </c>
       <c r="H113">
-        <f t="shared" ref="H113:I113" si="111">AVERAGE(B113:B132)</f>
-        <v>2.5673995227434996</v>
+        <f t="shared" ref="H113:I113" si="111">AVERAGE(B113:B122)</f>
+        <v>2.370636380399</v>
       </c>
       <c r="I113">
         <f t="shared" si="111"/>
-        <v>-1.2131173053655</v>
+        <v>-0.17646342127799999</v>
       </c>
       <c r="J113">
         <v>-2.3274264317064999</v>
@@ -6957,12 +6959,12 @@
         <v>-1.1912230486140001</v>
       </c>
       <c r="H114">
-        <f t="shared" ref="H114:I114" si="112">AVERAGE(B114:B133)</f>
-        <v>2.8672401300109991</v>
+        <f t="shared" ref="H114:I114" si="112">AVERAGE(B114:B123)</f>
+        <v>3.2273008119959998</v>
       </c>
       <c r="I114">
         <f t="shared" si="112"/>
-        <v>-1.1912230486140001</v>
+        <v>-0.74813994768100001</v>
       </c>
       <c r="J114">
         <v>-2.4212296162744997</v>
@@ -6985,12 +6987,12 @@
         <v>-1.0426461916135001</v>
       </c>
       <c r="H115">
-        <f t="shared" ref="H115:I115" si="113">AVERAGE(B115:B134)</f>
-        <v>2.8020376184264992</v>
+        <f t="shared" ref="H115:I115" si="113">AVERAGE(B115:B124)</f>
+        <v>2.9821791913829996</v>
       </c>
       <c r="I115">
         <f t="shared" si="113"/>
-        <v>-1.0426461916135001</v>
+        <v>-6.7055348413000093E-2</v>
       </c>
       <c r="J115">
         <v>-2.4284677180979997</v>
@@ -7013,12 +7015,12 @@
         <v>-1.0202645915760002</v>
       </c>
       <c r="H116">
-        <f t="shared" ref="H116:I116" si="114">AVERAGE(B116:B135)</f>
-        <v>2.8145377147249997</v>
+        <f t="shared" ref="H116:I116" si="114">AVERAGE(B116:B125)</f>
+        <v>2.7077886970679996</v>
       </c>
       <c r="I116">
         <f t="shared" si="114"/>
-        <v>-1.0202645915760002</v>
+        <v>-0.40792128667300015</v>
       </c>
       <c r="J116">
         <v>-2.4309150407805</v>
@@ -7041,12 +7043,12 @@
         <v>-1.1192483780090001</v>
       </c>
       <c r="H117">
-        <f t="shared" ref="H117:I117" si="115">AVERAGE(B117:B136)</f>
-        <v>2.8510479778215001</v>
+        <f t="shared" ref="H117:I117" si="115">AVERAGE(B117:B126)</f>
+        <v>2.727289870491</v>
       </c>
       <c r="I117">
         <f t="shared" si="115"/>
-        <v>-1.1192483780090001</v>
+        <v>-0.40600839946</v>
       </c>
       <c r="J117">
         <v>-2.4138282441505003</v>
@@ -7069,12 +7071,12 @@
         <v>-1.1246953314730002</v>
       </c>
       <c r="H118">
-        <f t="shared" ref="H118:I118" si="116">AVERAGE(B118:B137)</f>
-        <v>2.8531872670055001</v>
+        <f t="shared" ref="H118:I118" si="116">AVERAGE(B118:B127)</f>
+        <v>2.5107027291390001</v>
       </c>
       <c r="I118">
         <f t="shared" si="116"/>
-        <v>-1.1246953314730002</v>
+        <v>-0.87766954019900001</v>
       </c>
       <c r="J118">
         <v>-2.419227197908</v>
@@ -7097,12 +7099,12 @@
         <v>-1.0817809225605002</v>
       </c>
       <c r="H119">
-        <f t="shared" ref="H119:I119" si="117">AVERAGE(B119:B138)</f>
-        <v>2.8370101163144996</v>
+        <f t="shared" ref="H119:I119" si="117">AVERAGE(B119:B128)</f>
+        <v>2.5483631336670003</v>
       </c>
       <c r="I119">
         <f t="shared" si="117"/>
-        <v>-1.0817809225605002</v>
+        <v>-0.98163559811300005</v>
       </c>
       <c r="J119">
         <v>-2.4217394505045</v>
@@ -7125,12 +7127,12 @@
         <v>-1.2338547063645</v>
       </c>
       <c r="H120">
-        <f t="shared" ref="H120:I120" si="118">AVERAGE(B120:B139)</f>
-        <v>2.8644498347524996</v>
+        <f t="shared" ref="H120:I120" si="118">AVERAGE(B120:B129)</f>
+        <v>2.5557122693149998</v>
       </c>
       <c r="I120">
         <f t="shared" si="118"/>
-        <v>-1.2338547063645</v>
+        <v>-1.1579419995490001</v>
       </c>
       <c r="J120">
         <v>-2.4113423492665005</v>
@@ -7153,12 +7155,12 @@
         <v>-1.2336904427549999</v>
       </c>
       <c r="H121">
-        <f t="shared" ref="H121:I121" si="119">AVERAGE(B121:B140)</f>
-        <v>2.8637449066705001</v>
+        <f t="shared" ref="H121:I121" si="119">AVERAGE(B121:B130)</f>
+        <v>2.34111017165</v>
       </c>
       <c r="I121">
         <f t="shared" si="119"/>
-        <v>-1.2336904427549999</v>
+        <v>-1.4784886520299998</v>
       </c>
       <c r="J121">
         <v>-2.4136791207945003</v>
@@ -7181,12 +7183,12 @@
         <v>-1.0812067709800002</v>
       </c>
       <c r="H122">
-        <f t="shared" ref="H122:I122" si="120">AVERAGE(B122:B141)</f>
-        <v>2.8065465104345</v>
+        <f t="shared" ref="H122:I122" si="120">AVERAGE(B122:B131)</f>
+        <v>2.6460692522830001</v>
       </c>
       <c r="I122">
         <f t="shared" si="120"/>
-        <v>-1.0812067709800002</v>
+        <v>-1.8557236675650004</v>
       </c>
       <c r="J122">
         <v>-2.4187825239664997</v>
@@ -7209,12 +7211,12 @@
         <v>-1.0481584241815001</v>
       </c>
       <c r="H123">
-        <f t="shared" ref="H123:I123" si="121">AVERAGE(B123:B142)</f>
-        <v>2.9028297482804999</v>
+        <f t="shared" ref="H123:I123" si="121">AVERAGE(B123:B132)</f>
+        <v>2.764162665088</v>
       </c>
       <c r="I123">
         <f t="shared" si="121"/>
-        <v>-1.0481584241815001</v>
+        <v>-2.2497711894530004</v>
       </c>
       <c r="J123">
         <v>-2.4559282157455002</v>
@@ -7237,12 +7239,12 @@
         <v>-0.86130688467599992</v>
       </c>
       <c r="H124">
-        <f t="shared" ref="H124:I124" si="122">AVERAGE(B124:B143)</f>
-        <v>2.8190938580104996</v>
+        <f t="shared" ref="H124:I124" si="122">AVERAGE(B124:B133)</f>
+        <v>2.5071794480260001</v>
       </c>
       <c r="I124">
         <f t="shared" si="122"/>
-        <v>-0.86130688467599992</v>
+        <v>-1.6343061495469999</v>
       </c>
       <c r="J124">
         <v>-2.477347529102</v>
@@ -7265,12 +7267,12 @@
         <v>-1.2820512123515002</v>
       </c>
       <c r="H125">
-        <f t="shared" ref="H125:I125" si="123">AVERAGE(B125:B144)</f>
-        <v>2.6509953662374999</v>
+        <f t="shared" ref="H125:I125" si="123">AVERAGE(B125:B134)</f>
+        <v>2.6218960454699998</v>
       </c>
       <c r="I125">
         <f t="shared" si="123"/>
-        <v>-1.2820512123515002</v>
+        <v>-2.0182370348140002</v>
       </c>
       <c r="J125">
         <v>-2.7617254802884998</v>
@@ -7293,12 +7295,12 @@
         <v>-1.1404460208855001</v>
       </c>
       <c r="H126">
-        <f t="shared" ref="H126:I126" si="124">AVERAGE(B126:B145)</f>
-        <v>2.8036438921264994</v>
+        <f t="shared" ref="H126:I126" si="124">AVERAGE(B126:B135)</f>
+        <v>2.9212867323819998</v>
       </c>
       <c r="I126">
         <f t="shared" si="124"/>
-        <v>-1.1404460208855001</v>
+        <v>-1.6326078964790001</v>
       </c>
       <c r="J126">
         <v>-2.7637054782369996</v>
@@ -7321,12 +7323,12 @@
         <v>-1.4868326801255001</v>
       </c>
       <c r="H127">
-        <f t="shared" ref="H127:I127" si="125">AVERAGE(B127:B146)</f>
-        <v>2.9664211646535001</v>
+        <f t="shared" ref="H127:I127" si="125">AVERAGE(B127:B136)</f>
+        <v>2.9748060851520002</v>
       </c>
       <c r="I127">
         <f t="shared" si="125"/>
-        <v>-1.4868326801255001</v>
+        <v>-1.8324883565580001</v>
       </c>
       <c r="J127">
         <v>-2.9282875879970001</v>
@@ -7349,12 +7351,12 @@
         <v>-1.2510521484474999</v>
       </c>
       <c r="H128">
-        <f t="shared" ref="H128:I128" si="126">AVERAGE(B128:B147)</f>
-        <v>3.0747111059505001</v>
+        <f t="shared" ref="H128:I128" si="126">AVERAGE(B128:B137)</f>
+        <v>3.1956718048720001</v>
       </c>
       <c r="I128">
         <f t="shared" si="126"/>
-        <v>-1.2510521484474999</v>
+        <v>-1.3717211227469999</v>
       </c>
       <c r="J128">
         <v>-2.9149397146145</v>
@@ -7377,12 +7379,12 @@
         <v>-1.1561547106065002</v>
       </c>
       <c r="H129">
-        <f t="shared" ref="H129:I129" si="127">AVERAGE(B129:B148)</f>
-        <v>3.0397037529935003</v>
+        <f t="shared" ref="H129:I129" si="127">AVERAGE(B129:B138)</f>
+        <v>3.1256570989620003</v>
       </c>
       <c r="I129">
         <f t="shared" si="127"/>
-        <v>-1.1561547106065002</v>
+        <v>-1.1819262470080001</v>
       </c>
       <c r="J129">
         <v>-2.754785584665</v>
@@ -7405,12 +7407,12 @@
         <v>-1.2660672108909998</v>
       </c>
       <c r="H130">
-        <f t="shared" ref="H130:I130" si="128">AVERAGE(B130:B149)</f>
-        <v>3.0803074996110005</v>
+        <f t="shared" ref="H130:I130" si="128">AVERAGE(B130:B139)</f>
+        <v>3.1731874001900002</v>
       </c>
       <c r="I130">
         <f t="shared" si="128"/>
-        <v>-1.2660672108909998</v>
+        <v>-1.3097674131799999</v>
       </c>
       <c r="J130">
         <v>-2.65205060042</v>
@@ -7433,12 +7435,12 @@
         <v>-1.1056693081145001</v>
       </c>
       <c r="H131">
-        <f t="shared" ref="H131:I131" si="129">AVERAGE(B131:B150)</f>
-        <v>3.1869073692695</v>
+        <f t="shared" ref="H131:I131" si="129">AVERAGE(B131:B140)</f>
+        <v>3.3863796416909997</v>
       </c>
       <c r="I131">
         <f t="shared" si="129"/>
-        <v>-1.1056693081145001</v>
+        <v>-0.98889223347999999</v>
       </c>
       <c r="J131">
         <v>-2.7786307165310005</v>
@@ -7461,12 +7463,12 @@
         <v>-0.82575099097699989</v>
       </c>
       <c r="H132">
-        <f t="shared" ref="H132:I132" si="130">AVERAGE(B132:B151)</f>
-        <v>2.9998501723475006</v>
+        <f t="shared" ref="H132:I132" si="130">AVERAGE(B132:B141)</f>
+        <v>2.9670237685860004</v>
       </c>
       <c r="I132">
         <f t="shared" si="130"/>
-        <v>-0.82575099097699989</v>
+        <v>-0.30668987439499984</v>
       </c>
       <c r="J132">
         <v>-2.7371895509755002</v>
@@ -7489,12 +7491,12 @@
         <v>-0.59567888323449991</v>
       </c>
       <c r="H133">
-        <f t="shared" ref="H133:I133" si="131">AVERAGE(B133:B152)</f>
-        <v>3.0370867037910001</v>
+        <f t="shared" ref="H133:I133" si="131">AVERAGE(B133:B142)</f>
+        <v>3.0414968314729998</v>
       </c>
       <c r="I133">
         <f t="shared" si="131"/>
-        <v>-0.59567888323449991</v>
+        <v>0.15345434109</v>
       </c>
       <c r="J133">
         <v>-2.6283268189610003</v>
@@ -7517,12 +7519,12 @@
         <v>-0.59566763936249989</v>
       </c>
       <c r="H134">
-        <f t="shared" ref="H134:I134" si="132">AVERAGE(B134:B153)</f>
-        <v>3.0370875197635003</v>
+        <f t="shared" ref="H134:I134" si="132">AVERAGE(B134:B143)</f>
+        <v>3.131008267995</v>
       </c>
       <c r="I134">
         <f t="shared" si="132"/>
-        <v>-0.59566763936249989</v>
+        <v>-8.8307619804999987E-2</v>
       </c>
       <c r="J134">
         <v>-2.5401910323940005</v>
@@ -7545,12 +7547,12 @@
         <v>-0.33620246592850006</v>
       </c>
       <c r="H135">
-        <f t="shared" ref="H135:I135" si="133">AVERAGE(B135:B154)</f>
-        <v>2.8107657279214999</v>
+        <f t="shared" ref="H135:I135" si="133">AVERAGE(B135:B144)</f>
+        <v>2.680094687005</v>
       </c>
       <c r="I135">
         <f t="shared" si="133"/>
-        <v>-0.33620246592850006</v>
+        <v>-0.54586538988900002</v>
       </c>
       <c r="J135">
         <v>-2.5449508904684999</v>
@@ -7573,12 +7575,12 @@
         <v>-0.3563883379704999</v>
       </c>
       <c r="H136">
-        <f t="shared" ref="H136:I136" si="134">AVERAGE(B136:B155)</f>
-        <v>2.8035891742300003</v>
+        <f t="shared" ref="H136:I136" si="134">AVERAGE(B136:B145)</f>
+        <v>2.686001051871</v>
       </c>
       <c r="I136">
         <f t="shared" si="134"/>
-        <v>-0.3563883379704999</v>
+        <v>-0.64828414529199996</v>
       </c>
       <c r="J136">
         <v>-2.5639725493590002</v>
@@ -7601,12 +7603,12 @@
         <v>-0.25740457821350005</v>
       </c>
       <c r="H137">
-        <f t="shared" ref="H137:I137" si="135">AVERAGE(B137:B156)</f>
-        <v>2.7670789085325</v>
+        <f t="shared" ref="H137:I137" si="135">AVERAGE(B137:B146)</f>
+        <v>2.9580362441550001</v>
       </c>
       <c r="I137">
         <f t="shared" si="135"/>
-        <v>-0.25740457821350005</v>
+        <v>-1.141177003693</v>
       </c>
       <c r="J137">
         <v>-2.3647784698335004</v>
@@ -7629,12 +7631,12 @@
         <v>-0.34489939717249996</v>
       </c>
       <c r="H138">
-        <f t="shared" ref="H138:I138" si="136">AVERAGE(B138:B157)</f>
-        <v>2.7992097534334994</v>
+        <f t="shared" ref="H138:I138" si="136">AVERAGE(B138:B147)</f>
+        <v>2.9537504070289993</v>
       </c>
       <c r="I138">
         <f t="shared" si="136"/>
-        <v>-0.34489939717249996</v>
+        <v>-1.1303831741479999</v>
       </c>
       <c r="J138">
         <v>-2.1716222571719999</v>
@@ -7657,12 +7659,12 @@
         <v>-0.34489130224850001</v>
       </c>
       <c r="H139">
-        <f t="shared" ref="H139:I139" si="137">AVERAGE(B139:B158)</f>
-        <v>2.7992105426315002</v>
+        <f t="shared" ref="H139:I139" si="137">AVERAGE(B139:B148)</f>
+        <v>2.9537504070249998</v>
       </c>
       <c r="I139">
         <f t="shared" si="137"/>
-        <v>-0.34489130224850001</v>
+        <v>-1.1303831742050001</v>
       </c>
       <c r="J139">
         <v>-1.9327888424359998</v>
@@ -7685,12 +7687,12 @@
         <v>-0.36199567267549998</v>
       </c>
       <c r="H140">
-        <f t="shared" ref="H140:I140" si="138">AVERAGE(B140:B159)</f>
-        <v>2.5179909633819997</v>
+        <f t="shared" ref="H140:I140" si="138">AVERAGE(B140:B149)</f>
+        <v>2.9874275990319998</v>
       </c>
       <c r="I140">
         <f t="shared" si="138"/>
-        <v>-0.36199567267549998</v>
+        <v>-1.222367008602</v>
       </c>
       <c r="J140">
         <v>-1.7369485910364997</v>
@@ -7713,12 +7715,12 @@
         <v>-0.52514686892649998</v>
       </c>
       <c r="H141">
-        <f t="shared" ref="H141:I141" si="139">AVERAGE(B141:B160)</f>
-        <v>2.4659494044904999</v>
+        <f t="shared" ref="H141:I141" si="139">AVERAGE(B141:B150)</f>
+        <v>2.9874350968479999</v>
       </c>
       <c r="I141">
         <f t="shared" si="139"/>
-        <v>-0.52514686892649998</v>
+        <v>-1.2224463827489997</v>
       </c>
       <c r="J141">
         <v>-1.5536150860839997</v>
@@ -7741,12 +7743,12 @@
         <v>-0.52549012043200005</v>
       </c>
       <c r="H142">
-        <f t="shared" ref="H142:I142" si="140">AVERAGE(B142:B161)</f>
-        <v>2.4659203476229998</v>
+        <f t="shared" ref="H142:I142" si="140">AVERAGE(B142:B151)</f>
+        <v>3.032676576109</v>
       </c>
       <c r="I142">
         <f t="shared" si="140"/>
-        <v>-0.52549012043200005</v>
+        <v>-1.3448121075589998</v>
       </c>
       <c r="J142">
         <v>-1.3081315450675</v>
@@ -7769,12 +7771,12 @@
         <v>-0.52547851941099988</v>
       </c>
       <c r="H143">
-        <f t="shared" ref="H143:I143" si="141">AVERAGE(B143:B162)</f>
-        <v>2.4659211895094999</v>
+        <f t="shared" ref="H143:I143" si="141">AVERAGE(B143:B152)</f>
+        <v>3.032676576109</v>
       </c>
       <c r="I143">
         <f t="shared" si="141"/>
-        <v>-0.52547851941099988</v>
+        <v>-1.3448121075589998</v>
       </c>
       <c r="J143">
         <v>-1.1877845079674998</v>
@@ -7797,12 +7799,12 @@
         <v>-0.40458609313900001</v>
       </c>
       <c r="H144">
-        <f t="shared" ref="H144:I144" si="142">AVERAGE(B144:B163)</f>
-        <v>2.4211663018739999</v>
+        <f t="shared" ref="H144:I144" si="142">AVERAGE(B144:B153)</f>
+        <v>2.9431667715319998</v>
       </c>
       <c r="I144">
         <f t="shared" si="142"/>
-        <v>-0.40458609313900001</v>
+        <v>-1.1030276589199999</v>
       </c>
       <c r="J144">
         <v>-0.99285063743900026</v>
@@ -7825,12 +7827,12 @@
         <v>-0.16082975856899998</v>
       </c>
       <c r="H145">
-        <f t="shared" ref="H145:I145" si="143">AVERAGE(B145:B164)</f>
-        <v>2.6407940728435002</v>
+        <f t="shared" ref="H145:I145" si="143">AVERAGE(B145:B154)</f>
+        <v>2.9414367688379999</v>
       </c>
       <c r="I145">
         <f t="shared" si="143"/>
-        <v>-0.16082975856899998</v>
+        <v>-0.12653954196799999</v>
       </c>
       <c r="J145">
         <v>-0.77856059181850024</v>
@@ -7853,12 +7855,12 @@
         <v>-0.14361379841950001</v>
       </c>
       <c r="H146">
-        <f t="shared" ref="H146:I146" si="144">AVERAGE(B146:B165)</f>
-        <v>2.6343031416409999</v>
+        <f t="shared" ref="H146:I146" si="144">AVERAGE(B146:B155)</f>
+        <v>2.9211772965889997</v>
       </c>
       <c r="I146">
         <f t="shared" si="144"/>
-        <v>-0.14361379841950001</v>
+        <v>-6.4492530648999957E-2</v>
       </c>
       <c r="J146">
         <v>-0.59668660013949992</v>
@@ -7881,12 +7883,12 @@
         <v>7.7893408353499977E-2</v>
       </c>
       <c r="H147">
-        <f t="shared" ref="H147:I147" si="145">AVERAGE(B147:B166)</f>
-        <v>2.5077037881105002</v>
+        <f t="shared" ref="H147:I147" si="145">AVERAGE(B147:B156)</f>
+        <v>2.57612157291</v>
       </c>
       <c r="I147">
         <f t="shared" si="145"/>
-        <v>7.7893408353499977E-2</v>
+        <v>0.62636784726599992</v>
       </c>
       <c r="J147">
         <v>-0.36466994545900011</v>
@@ -7909,12 +7911,12 @@
         <v>-5.0059312043999979E-2</v>
       </c>
       <c r="H148">
-        <f t="shared" ref="H148:I148" si="146">AVERAGE(B148:B167)</f>
-        <v>2.5551950252445002</v>
+        <f t="shared" ref="H148:I148" si="146">AVERAGE(B148:B157)</f>
+        <v>2.6446690998380005</v>
       </c>
       <c r="I148">
         <f t="shared" si="146"/>
-        <v>-5.0059312043999979E-2</v>
+        <v>0.44058437980300003</v>
       </c>
       <c r="J148">
         <v>-3.7703310485499998E-2</v>
@@ -7937,12 +7939,12 @@
         <v>-0.18012359231549999</v>
       </c>
       <c r="H149">
-        <f t="shared" ref="H149:I149" si="147">AVERAGE(B149:B168)</f>
-        <v>2.6035112560335003</v>
+        <f t="shared" ref="H149:I149" si="147">AVERAGE(B149:B158)</f>
+        <v>2.6446706782380001</v>
       </c>
       <c r="I149">
         <f t="shared" si="147"/>
-        <v>-0.18012359231549999</v>
+        <v>0.44060056970800004</v>
       </c>
       <c r="J149">
         <v>-1.8250996808500029E-2</v>
@@ -7965,12 +7967,12 @@
         <v>-0.20191087576300001</v>
       </c>
       <c r="H150">
-        <f t="shared" ref="H150:I150" si="148">AVERAGE(B150:B169)</f>
-        <v>2.6118646453194998</v>
+        <f t="shared" ref="H150:I150" si="148">AVERAGE(B150:B159)</f>
+        <v>2.048554327732</v>
       </c>
       <c r="I150">
         <f t="shared" si="148"/>
-        <v>-0.20191087576300001</v>
+        <v>0.49837566325100002</v>
       </c>
       <c r="J150">
         <v>7.7555340735499897E-2</v>
@@ -7993,12 +7995,12 @@
         <v>-0.33487415243000002</v>
       </c>
       <c r="H151">
-        <f t="shared" ref="H151:I151" si="149">AVERAGE(B151:B170)</f>
-        <v>2.6613124260930001</v>
+        <f t="shared" ref="H151:I151" si="149">AVERAGE(B151:B160)</f>
+        <v>1.944463712133</v>
       </c>
       <c r="I151">
         <f t="shared" si="149"/>
-        <v>-0.33487415243000002</v>
+        <v>0.17215264489599996</v>
       </c>
       <c r="J151">
         <v>0.21183605127150007</v>
@@ -8021,12 +8023,12 @@
         <v>-0.39306028789200004</v>
       </c>
       <c r="H152">
-        <f t="shared" ref="H152:I152" si="150">AVERAGE(B152:B171)</f>
-        <v>2.682703405971</v>
+        <f t="shared" ref="H152:I152" si="150">AVERAGE(B152:B161)</f>
+        <v>1.8991641191370001</v>
       </c>
       <c r="I152">
         <f t="shared" si="150"/>
-        <v>-0.39306028789200004</v>
+        <v>0.29383186669499994</v>
       </c>
       <c r="J152">
         <v>0.15992400448999994</v>
@@ -8049,12 +8051,12 @@
         <v>-0.52237978371600002</v>
       </c>
       <c r="H153">
-        <f t="shared" ref="H153:I153" si="151">AVERAGE(B153:B172)</f>
-        <v>2.7307279886250004</v>
+        <f t="shared" ref="H153:I153" si="151">AVERAGE(B153:B162)</f>
+        <v>1.8991658029100003</v>
       </c>
       <c r="I153">
         <f t="shared" si="151"/>
-        <v>-0.52237978371600002</v>
+        <v>0.29385506873700001</v>
       </c>
       <c r="J153">
         <v>0.25057457387600002</v>
@@ -8077,12 +8079,12 @@
         <v>-0.61331992886499997</v>
       </c>
       <c r="H154">
-        <f t="shared" ref="H154:I154" si="152">AVERAGE(B154:B173)</f>
-        <v>2.7642790343220001</v>
+        <f t="shared" ref="H154:I154" si="152">AVERAGE(B154:B163)</f>
+        <v>1.8991658322159999</v>
       </c>
       <c r="I154">
         <f t="shared" si="152"/>
-        <v>-0.61331992886499997</v>
+        <v>0.29385547264200002</v>
       </c>
       <c r="J154">
         <v>0.5262558734635</v>
@@ -8105,12 +8107,12 @@
         <v>-0.97193386223949996</v>
       </c>
       <c r="H155">
-        <f t="shared" ref="H155:I155" si="153">AVERAGE(B155:B174)</f>
-        <v>3.0269466193125005</v>
+        <f t="shared" ref="H155:I155" si="153">AVERAGE(B155:B164)</f>
+        <v>2.3401513768489997</v>
       </c>
       <c r="I155">
         <f t="shared" si="153"/>
-        <v>-0.97193386223949996</v>
+        <v>-0.19511997516999999</v>
       </c>
       <c r="J155">
         <v>0.50674390745399989</v>
@@ -8133,12 +8135,12 @@
         <v>-1.0845608261499999</v>
       </c>
       <c r="H156">
-        <f t="shared" ref="H156:I156" si="154">AVERAGE(B156:B175)</f>
-        <v>3.0668281651719997</v>
+        <f t="shared" ref="H156:I156" si="154">AVERAGE(B156:B165)</f>
+        <v>2.347428986693</v>
       </c>
       <c r="I156">
         <f t="shared" si="154"/>
-        <v>-1.0845608261499999</v>
+        <v>-0.22273506618999997</v>
       </c>
       <c r="J156">
         <v>0.76116938298150005</v>
@@ -8161,12 +8163,12 @@
         <v>-1.2767258058109998</v>
       </c>
       <c r="H157">
-        <f t="shared" ref="H157:I157" si="155">AVERAGE(B157:B176)</f>
-        <v>3.1447176050985002</v>
+        <f t="shared" ref="H157:I157" si="155">AVERAGE(B157:B166)</f>
+        <v>2.439286003311</v>
       </c>
       <c r="I157">
         <f t="shared" si="155"/>
-        <v>-1.2767258058109998</v>
+        <v>-0.47058103055899991</v>
       </c>
       <c r="J157">
         <v>0.62166479737949998</v>
@@ -8189,12 +8191,12 @@
         <v>-1.1285556902209999</v>
       </c>
       <c r="H158">
-        <f t="shared" ref="H158:I158" si="156">AVERAGE(B158:B177)</f>
-        <v>3.1107039614164997</v>
+        <f t="shared" ref="H158:I158" si="156">AVERAGE(B158:B167)</f>
+        <v>2.4657209506509998</v>
       </c>
       <c r="I158">
         <f t="shared" si="156"/>
-        <v>-1.1285556902209999</v>
+        <v>-0.5407030038909999</v>
       </c>
       <c r="J158">
         <v>0.67474003421849982</v>
@@ -8217,12 +8219,12 @@
         <v>-0.91061650210900003</v>
       </c>
       <c r="H159">
-        <f t="shared" ref="H159:I159" si="157">AVERAGE(B159:B178)</f>
-        <v>3.0290257145634998</v>
+        <f t="shared" ref="H159:I159" si="157">AVERAGE(B159:B168)</f>
+        <v>2.5623518338290001</v>
       </c>
       <c r="I159">
         <f t="shared" si="157"/>
-        <v>-0.91061650210900003</v>
+        <v>-0.80084775433900002</v>
       </c>
       <c r="J159">
         <v>0.61677351175450001</v>
@@ -8245,12 +8247,12 @@
         <v>-0.64494006856450015</v>
       </c>
       <c r="H160">
-        <f t="shared" ref="H160:I160" si="158">AVERAGE(B160:B179)</f>
-        <v>3.2429991807710001</v>
+        <f t="shared" ref="H160:I160" si="158">AVERAGE(B160:B169)</f>
+        <v>3.1751749629070001</v>
       </c>
       <c r="I160">
         <f t="shared" si="158"/>
-        <v>-0.64494006856450015</v>
+        <v>-0.90219741477700011</v>
       </c>
       <c r="J160">
         <v>0.61350921480749998</v>
@@ -8273,12 +8275,12 @@
         <v>-0.20214135284150009</v>
       </c>
       <c r="H161">
-        <f t="shared" ref="H161:I161" si="159">AVERAGE(B161:B180)</f>
-        <v>3.1488073022774996</v>
+        <f t="shared" ref="H161:I161" si="159">AVERAGE(B161:B170)</f>
+        <v>3.3781611400529998</v>
       </c>
       <c r="I161">
         <f t="shared" si="159"/>
-        <v>-0.20214135284150009</v>
+        <v>-0.84190094975600016</v>
       </c>
       <c r="J161">
         <v>0.55144368933799981</v>
@@ -8301,12 +8303,12 @@
         <v>-0.22644491770049999</v>
       </c>
       <c r="H162">
-        <f t="shared" ref="H162:I162" si="160">AVERAGE(B162:B181)</f>
-        <v>3.1581547303269994</v>
+        <f t="shared" ref="H162:I162" si="160">AVERAGE(B162:B171)</f>
+        <v>3.4662426928050003</v>
       </c>
       <c r="I162">
         <f t="shared" si="160"/>
-        <v>-0.22644491770049999</v>
+        <v>-1.0799524424790001</v>
       </c>
       <c r="J162">
         <v>0.50885256945049995</v>
@@ -8329,12 +8331,12 @@
         <v>-0.4627165935955001</v>
       </c>
       <c r="H163">
-        <f t="shared" ref="H163:I163" si="161">AVERAGE(B163:B182)</f>
-        <v>3.1040734003094999</v>
+        <f t="shared" ref="H163:I163" si="161">AVERAGE(B163:B172)</f>
+        <v>3.5622901743400002</v>
       </c>
       <c r="I163">
         <f t="shared" si="161"/>
-        <v>-0.4627165935955001</v>
+        <v>-1.3386146361690001</v>
       </c>
       <c r="J163">
         <v>0.45200014614399986</v>
@@ -8357,12 +8359,12 @@
         <v>-0.46271312955350002</v>
       </c>
       <c r="H164">
-        <f t="shared" ref="H164:I164" si="162">AVERAGE(B164:B183)</f>
-        <v>3.1040736516339997</v>
+        <f t="shared" ref="H164:I164" si="162">AVERAGE(B164:B173)</f>
+        <v>3.629392236428</v>
       </c>
       <c r="I164">
         <f t="shared" si="162"/>
-        <v>-0.46271312955350002</v>
+        <v>-1.5204953303719999</v>
       </c>
       <c r="J164">
         <v>0.43814564050850002</v>
@@ -8385,12 +8387,12 @@
         <v>-0.49584292539300012</v>
       </c>
       <c r="H165">
-        <f t="shared" ref="H165:I165" si="163">AVERAGE(B165:B184)</f>
-        <v>3.1166831201715004</v>
+        <f t="shared" ref="H165:I165" si="163">AVERAGE(B165:B174)</f>
+        <v>3.7137418617760005</v>
       </c>
       <c r="I165">
         <f t="shared" si="163"/>
-        <v>-0.49584292539300012</v>
+        <v>-1.748747749309</v>
       </c>
       <c r="J165">
         <v>0.41240845937299991</v>
@@ -8413,12 +8415,12 @@
         <v>-0.58101830790150022</v>
       </c>
       <c r="H166">
-        <f t="shared" ref="H166:I166" si="164">AVERAGE(B166:B185)</f>
-        <v>3.1478565312759996</v>
+        <f t="shared" ref="H166:I166" si="164">AVERAGE(B166:B175)</f>
+        <v>3.7862273436509994</v>
       </c>
       <c r="I166">
         <f t="shared" si="164"/>
-        <v>-0.58101830790150022</v>
+        <v>-1.94638658611</v>
       </c>
       <c r="J166">
         <v>0.40586404882900001</v>
@@ -8441,12 +8443,12 @@
         <v>-0.4841294976190002</v>
       </c>
       <c r="H167">
-        <f t="shared" ref="H167:I167" si="165">AVERAGE(B167:B186)</f>
-        <v>3.1124015796899998</v>
+        <f t="shared" ref="H167:I167" si="165">AVERAGE(B167:B176)</f>
+        <v>3.8501492068859995</v>
       </c>
       <c r="I167">
         <f t="shared" si="165"/>
-        <v>-0.4841294976190002</v>
+        <v>-2.0828705810630002</v>
       </c>
       <c r="J167">
         <v>0.37715449297849996</v>
@@ -8469,12 +8471,12 @@
         <v>-0.42657665582900001</v>
       </c>
       <c r="H168">
-        <f t="shared" ref="H168:I168" si="166">AVERAGE(B168:B187)</f>
-        <v>3.0910031805374998</v>
+        <f t="shared" ref="H168:I168" si="166">AVERAGE(B168:B177)</f>
+        <v>3.7556869721820001</v>
       </c>
       <c r="I168">
         <f t="shared" si="166"/>
-        <v>-0.42657665582900001</v>
+        <v>-1.7164083765510001</v>
       </c>
       <c r="J168">
         <v>0.24220312174949993</v>
@@ -8497,12 +8499,12 @@
         <v>-0.39231605440250011</v>
       </c>
       <c r="H169">
-        <f t="shared" ref="H169:I169" si="167">AVERAGE(B169:B188)</f>
-        <v>3.0780285826160001</v>
+        <f t="shared" ref="H169:I169" si="167">AVERAGE(B169:B178)</f>
+        <v>3.4956995952980003</v>
       </c>
       <c r="I169">
         <f t="shared" si="167"/>
-        <v>-0.39231605440250011</v>
+        <v>-1.0203852498790003</v>
       </c>
       <c r="J169">
         <v>0.39318730465349994</v>
@@ -8525,12 +8527,12 @@
         <v>-0.49185377757949994</v>
       </c>
       <c r="H170">
-        <f t="shared" ref="H170:I170" si="168">AVERAGE(B170:B189)</f>
-        <v>3.125957366707</v>
+        <f t="shared" ref="H170:I170" si="168">AVERAGE(B170:B179)</f>
+        <v>3.3108233986350002</v>
       </c>
       <c r="I170">
         <f t="shared" si="168"/>
-        <v>-0.49185377757949994</v>
+        <v>-0.38768272235199985</v>
       </c>
       <c r="J170">
         <v>0.49451453547949997</v>
@@ -8553,12 +8555,12 @@
         <v>-0.49525535225950013</v>
       </c>
       <c r="H171">
-        <f t="shared" ref="H171:I171" si="169">AVERAGE(B171:B190)</f>
-        <v>3.0660930670425004</v>
+        <f t="shared" ref="H171:I171" si="169">AVERAGE(B171:B180)</f>
+        <v>2.9194534645020003</v>
       </c>
       <c r="I171">
         <f t="shared" si="169"/>
-        <v>-0.49525535225950013</v>
+        <v>0.43761824407299993</v>
       </c>
       <c r="J171">
         <v>0.53577879846199994</v>
@@ -8581,12 +8583,12 @@
         <v>-0.45398832391150012</v>
       </c>
       <c r="H172">
-        <f t="shared" ref="H172:I172" si="170">AVERAGE(B172:B191)</f>
-        <v>3.050805169452</v>
+        <f t="shared" ref="H172:I172" si="170">AVERAGE(B172:B181)</f>
+        <v>2.8500667678490004</v>
       </c>
       <c r="I172">
         <f t="shared" si="170"/>
-        <v>-0.45398832391150012</v>
+        <v>0.62706260707799988</v>
       </c>
       <c r="J172">
         <v>0.58768325844799996</v>
@@ -8609,12 +8611,12 @@
         <v>-0.3246324747655</v>
       </c>
       <c r="H173">
-        <f t="shared" ref="H173:I173" si="171">AVERAGE(B173:B192)</f>
-        <v>3.0027832238859999</v>
+        <f t="shared" ref="H173:I173" si="171">AVERAGE(B173:B182)</f>
+        <v>2.645856626279</v>
       </c>
       <c r="I173">
         <f t="shared" si="171"/>
-        <v>-0.3246324747655</v>
+        <v>0.41318144897800002</v>
       </c>
       <c r="J173">
         <v>0.58562451592749987</v>
@@ -8637,12 +8639,12 @@
         <v>-0.34709871055149993</v>
       </c>
       <c r="H174">
-        <f t="shared" ref="H174:I174" si="172">AVERAGE(B174:B193)</f>
-        <v>3.0111341027780001</v>
+        <f t="shared" ref="H174:I174" si="172">AVERAGE(B174:B183)</f>
+        <v>2.5787550668400003</v>
       </c>
       <c r="I174">
         <f t="shared" si="172"/>
-        <v>-0.34709871055149993</v>
+        <v>0.59506907126500008</v>
       </c>
       <c r="J174">
         <v>0.47780094302600001</v>
@@ -8665,12 +8667,12 @@
         <v>-0.23298629973199994</v>
       </c>
       <c r="H175">
-        <f t="shared" ref="H175:I175" si="173">AVERAGE(B175:B194)</f>
-        <v>2.9689582847155003</v>
+        <f t="shared" ref="H175:I175" si="173">AVERAGE(B175:B184)</f>
+        <v>2.5196243785669998</v>
       </c>
       <c r="I175">
         <f t="shared" si="173"/>
-        <v>-0.23298629973199994</v>
+        <v>0.7570618985230001</v>
       </c>
       <c r="J175">
         <v>0.59250952689649994</v>
@@ -8693,12 +8695,12 @@
         <v>-0.22362561570399997</v>
       </c>
       <c r="H176">
-        <f t="shared" ref="H176:I176" si="174">AVERAGE(B176:B195)</f>
-        <v>2.9654687419470003</v>
+        <f t="shared" ref="H176:I176" si="174">AVERAGE(B176:B185)</f>
+        <v>2.5094857189010003</v>
       </c>
       <c r="I176">
         <f t="shared" si="174"/>
-        <v>-0.22362561570399997</v>
+        <v>0.78434997030700004</v>
       </c>
       <c r="J176">
         <v>0.60268529720599995</v>
@@ -8721,12 +8723,12 @@
         <v>-3.1953834929499984E-2</v>
       </c>
       <c r="H177">
-        <f t="shared" ref="H177:I177" si="175">AVERAGE(B177:B196)</f>
-        <v>2.8877842403659999</v>
+        <f t="shared" ref="H177:I177" si="175">AVERAGE(B177:B186)</f>
+        <v>2.374653952494</v>
       </c>
       <c r="I177">
         <f t="shared" si="175"/>
-        <v>-3.1953834929499984E-2</v>
+        <v>1.1146115858250001</v>
       </c>
       <c r="J177">
         <v>0.72926816888250001</v>
@@ -8749,12 +8751,12 @@
         <v>-8.7232216797999959E-2</v>
       </c>
       <c r="H178">
-        <f t="shared" ref="H178:I178" si="176">AVERAGE(B178:B197)</f>
-        <v>2.887524120583</v>
+        <f t="shared" ref="H178:I178" si="176">AVERAGE(B178:B187)</f>
+        <v>2.4263193888929999</v>
       </c>
       <c r="I178">
         <f t="shared" si="176"/>
-        <v>-8.7232216797999959E-2</v>
+        <v>0.86325506489300019</v>
       </c>
       <c r="J178">
         <v>0.67157814994749987</v>
@@ -8777,12 +8779,12 @@
         <v>-0.46252413555049998</v>
       </c>
       <c r="H179">
-        <f t="shared" ref="H179:I179" si="177">AVERAGE(B179:B198)</f>
-        <v>3.0285647916715002</v>
+        <f t="shared" ref="H179:I179" si="177">AVERAGE(B179:B188)</f>
+        <v>2.6603575699339999</v>
       </c>
       <c r="I179">
         <f t="shared" si="177"/>
-        <v>-0.46252413555049998</v>
+        <v>0.23575314107400014</v>
       </c>
       <c r="J179">
         <v>0.72441778826199998</v>
@@ -8805,12 +8807,12 @@
         <v>-0.86501832754349994</v>
       </c>
       <c r="H180">
-        <f t="shared" ref="H180:I180" si="178">AVERAGE(B180:B199)</f>
-        <v>3.1435065789965</v>
+        <f t="shared" ref="H180:I180" si="178">AVERAGE(B180:B189)</f>
+        <v>2.9410913347790002</v>
       </c>
       <c r="I180">
         <f t="shared" si="178"/>
-        <v>-0.86501832754349994</v>
+        <v>-0.59602483280700014</v>
       </c>
       <c r="J180">
         <v>0.65983640698050006</v>
@@ -8833,12 +8835,12 @@
         <v>-1.1446926158330002</v>
       </c>
       <c r="H181">
-        <f t="shared" ref="H181:I181" si="179">AVERAGE(B181:B200)</f>
-        <v>3.2897380749710003</v>
+        <f t="shared" ref="H181:I181" si="179">AVERAGE(B181:B190)</f>
+        <v>3.2127326695830001</v>
       </c>
       <c r="I181">
         <f t="shared" si="179"/>
-        <v>-1.1446926158330002</v>
+        <v>-1.4281289485920001</v>
       </c>
       <c r="J181">
         <v>0.59570740235449993</v>
@@ -8861,12 +8863,12 @@
         <v>-1.2960574716350002</v>
       </c>
       <c r="H182">
-        <f t="shared" ref="H182:I182" si="180">AVERAGE(B182:B201)</f>
-        <v>3.3754003032170004</v>
+        <f t="shared" ref="H182:I182" si="180">AVERAGE(B182:B191)</f>
+        <v>3.251543571055</v>
       </c>
       <c r="I182">
         <f t="shared" si="180"/>
-        <v>-1.2960574716350002</v>
+        <v>-1.5350392549010001</v>
       </c>
       <c r="J182">
         <v>0.67086042731499995</v>
@@ -8889,12 +8891,12 @@
         <v>-1.1221444057534999</v>
       </c>
       <c r="H183">
-        <f t="shared" ref="H183:I183" si="181">AVERAGE(B183:B202)</f>
-        <v>3.4536316118745005</v>
+        <f t="shared" ref="H183:I183" si="181">AVERAGE(B183:B192)</f>
+        <v>3.3597098214929999</v>
       </c>
       <c r="I183">
         <f t="shared" si="181"/>
-        <v>-1.1221444057534999</v>
+        <v>-1.062446398509</v>
       </c>
       <c r="J183">
         <v>0.78836384353699995</v>
@@ -8917,12 +8919,12 @@
         <v>-1.1855166643454997</v>
       </c>
       <c r="H184">
-        <f t="shared" ref="H184:I184" si="182">AVERAGE(B184:B203)</f>
-        <v>3.4917891336220008</v>
+        <f t="shared" ref="H184:I184" si="182">AVERAGE(B184:B193)</f>
+        <v>3.4435131387160007</v>
       </c>
       <c r="I184">
         <f t="shared" si="182"/>
-        <v>-1.1855166643454997</v>
+        <v>-1.289266492368</v>
       </c>
       <c r="J184">
         <v>0.83017600572249983</v>
@@ -8945,12 +8947,12 @@
         <v>-1.3997390985604998</v>
       </c>
       <c r="H185">
-        <f t="shared" ref="H185:I185" si="183">AVERAGE(B185:B204)</f>
-        <v>3.6105878493770005</v>
+        <f t="shared" ref="H185:I185" si="183">AVERAGE(B185:B194)</f>
+        <v>3.4182921908639998</v>
       </c>
       <c r="I185">
         <f t="shared" si="183"/>
-        <v>-1.3997390985604998</v>
+        <v>-1.223034497987</v>
       </c>
       <c r="J185">
         <v>0.65995943661950007</v>
@@ -8973,12 +8975,12 @@
         <v>-1.4489820676224998</v>
       </c>
       <c r="H186">
-        <f t="shared" ref="H186:I186" si="184">AVERAGE(B186:B205)</f>
-        <v>3.6405209975040003</v>
+        <f t="shared" ref="H186:I186" si="184">AVERAGE(B186:B195)</f>
+        <v>3.4214517649930003</v>
       </c>
       <c r="I186">
         <f t="shared" si="184"/>
-        <v>-1.4489820676224998</v>
+        <v>-1.2316012017150002</v>
       </c>
       <c r="J186">
         <v>0.67104719343999997</v>
@@ -9001,12 +9003,12 @@
         <v>-1.4887359256434998</v>
       </c>
       <c r="H187">
-        <f t="shared" ref="H187:I187" si="185">AVERAGE(B187:B206)</f>
-        <v>3.6548450318049994</v>
+        <f t="shared" ref="H187:I187" si="185">AVERAGE(B187:B196)</f>
+        <v>3.4009145282379998</v>
       </c>
       <c r="I187">
         <f t="shared" si="185"/>
-        <v>-1.4887359256434998</v>
+        <v>-1.1785192556840003</v>
       </c>
       <c r="J187">
         <v>0.60837845582350014</v>
@@ -9029,12 +9031,12 @@
         <v>-1.3576400101939998</v>
       </c>
       <c r="H188">
-        <f t="shared" ref="H188:I188" si="186">AVERAGE(B188:B207)</f>
-        <v>3.6383982194879989</v>
+        <f t="shared" ref="H188:I188" si="186">AVERAGE(B188:B197)</f>
+        <v>3.3487288522729997</v>
       </c>
       <c r="I188">
         <f t="shared" si="186"/>
-        <v>-1.3576400101939998</v>
+        <v>-1.0377194984890001</v>
       </c>
       <c r="J188">
         <v>0.70898964926950014</v>
@@ -9057,12 +9059,12 @@
         <v>-1.3164417644224997</v>
       </c>
       <c r="H189">
-        <f t="shared" ref="H189:I189" si="187">AVERAGE(B189:B208)</f>
-        <v>3.638837732340499</v>
+        <f t="shared" ref="H189:I189" si="187">AVERAGE(B189:B198)</f>
+        <v>3.396772013409</v>
       </c>
       <c r="I189">
         <f t="shared" si="187"/>
-        <v>-1.3164417644224997</v>
+        <v>-1.1608014121749999</v>
       </c>
       <c r="J189">
         <v>0.6722460525895001</v>
@@ -9085,12 +9087,12 @@
         <v>-1.0959829764204998</v>
       </c>
       <c r="H190">
-        <f t="shared" ref="H190:I190" si="188">AVERAGE(B190:B209)</f>
-        <v>3.5461867136174989</v>
+        <f t="shared" ref="H190:I190" si="188">AVERAGE(B190:B199)</f>
+        <v>3.3459218232140002</v>
       </c>
       <c r="I190">
         <f t="shared" si="188"/>
-        <v>-1.0959829764204998</v>
+        <v>-1.1340118222800002</v>
       </c>
       <c r="J190">
         <v>0.67653188044250001</v>
@@ -9113,12 +9115,12 @@
         <v>-0.99515289550349983</v>
       </c>
       <c r="H191">
-        <f t="shared" ref="H191:I191" si="189">AVERAGE(B191:B210)</f>
-        <v>3.5700919706239995</v>
+        <f t="shared" ref="H191:I191" si="189">AVERAGE(B191:B200)</f>
+        <v>3.3667434803589997</v>
       </c>
       <c r="I191">
         <f t="shared" si="189"/>
-        <v>-0.99515289550349983</v>
+        <v>-0.86125628307400004</v>
       </c>
       <c r="J191">
         <v>0.78155695939049996</v>
@@ -9141,12 +9143,12 @@
         <v>-0.9173956885965</v>
       </c>
       <c r="H192">
-        <f t="shared" ref="H192:I192" si="190">AVERAGE(B192:B211)</f>
-        <v>3.5413389821975003</v>
+        <f t="shared" ref="H192:I192" si="190">AVERAGE(B192:B201)</f>
+        <v>3.4992570353790002</v>
       </c>
       <c r="I192">
         <f t="shared" si="190"/>
-        <v>-0.9173956885965</v>
+        <v>-1.057075688369</v>
       </c>
       <c r="J192">
         <v>0.84142924690950005</v>
@@ -9169,12 +9171,12 @@
         <v>-1.1469968567169999</v>
       </c>
       <c r="H193">
-        <f t="shared" ref="H193:I193" si="191">AVERAGE(B193:B212)</f>
-        <v>3.3259844154969995</v>
+        <f t="shared" ref="H193:I193" si="191">AVERAGE(B193:B202)</f>
+        <v>3.5475534022559998</v>
       </c>
       <c r="I193">
         <f t="shared" si="191"/>
-        <v>-1.1469968567169999</v>
+        <v>-1.1818424129980001</v>
       </c>
       <c r="J193">
         <v>0.95035299862</v>
@@ -9197,12 +9199,12 @@
         <v>-1.0989075403719999</v>
       </c>
       <c r="H194">
-        <f t="shared" ref="H194:I194" si="192">AVERAGE(B194:B213)</f>
-        <v>3.3170573124760003</v>
+        <f t="shared" ref="H194:I194" si="192">AVERAGE(B194:B203)</f>
+        <v>3.540065128528</v>
       </c>
       <c r="I194">
         <f t="shared" si="192"/>
-        <v>-1.0989075403719999</v>
+        <v>-1.081766836323</v>
       </c>
       <c r="J194">
         <v>1.0629004697160001</v>
@@ -9225,12 +9227,12 @@
         <v>-1.1933336534305004</v>
       </c>
       <c r="H195">
-        <f t="shared" ref="H195:I195" si="193">AVERAGE(B195:B214)</f>
-        <v>3.3518909141269999</v>
+        <f t="shared" ref="H195:I195" si="193">AVERAGE(B195:B204)</f>
+        <v>3.8028835078900003</v>
       </c>
       <c r="I195">
         <f t="shared" si="193"/>
-        <v>-1.1933336534305004</v>
+        <v>-1.5764436991340001</v>
       </c>
       <c r="J195">
         <v>1.2698482833740004</v>
@@ -9253,12 +9255,12 @@
         <v>-1.0726107961940001</v>
       </c>
       <c r="H196">
-        <f t="shared" ref="H196:I196" si="194">AVERAGE(B196:B215)</f>
-        <v>3.3325160816109998</v>
+        <f t="shared" ref="H196:I196" si="194">AVERAGE(B196:B205)</f>
+        <v>3.8595902300150002</v>
       </c>
       <c r="I196">
         <f t="shared" si="194"/>
-        <v>-1.0726107961940001</v>
+        <v>-1.6663629335299999</v>
       </c>
       <c r="J196">
         <v>1.2890774891500001</v>
@@ -9281,12 +9283,12 @@
         <v>-1.2353514133620003</v>
       </c>
       <c r="H197">
-        <f t="shared" ref="H197:I197" si="195">AVERAGE(B197:B216)</f>
-        <v>3.2527350772874994</v>
+        <f t="shared" ref="H197:I197" si="195">AVERAGE(B197:B206)</f>
+        <v>3.908775535372</v>
       </c>
       <c r="I197">
         <f t="shared" si="195"/>
-        <v>-1.2353514133620003</v>
+        <v>-1.7989525956029997</v>
       </c>
       <c r="J197">
         <v>1.3885014728830003</v>
@@ -9309,12 +9311,12 @@
         <v>-1.2353514133620003</v>
       </c>
       <c r="H198">
-        <f t="shared" ref="H198:I198" si="196">AVERAGE(B198:B217)</f>
-        <v>3.2527350772874994</v>
+        <f t="shared" ref="H198:I198" si="196">AVERAGE(B198:B207)</f>
+        <v>3.9280675867029999</v>
       </c>
       <c r="I198">
         <f t="shared" si="196"/>
-        <v>-1.2353514133620003</v>
+        <v>-1.6775605218989997</v>
       </c>
       <c r="J198">
         <v>1.6605291132545001</v>
@@ -9337,12 +9339,12 @@
         <v>-1.1513285456590006</v>
       </c>
       <c r="H199">
-        <f t="shared" ref="H199:I199" si="197">AVERAGE(B199:B218)</f>
-        <v>3.2205278463285003</v>
+        <f t="shared" ref="H199:I199" si="197">AVERAGE(B199:B208)</f>
+        <v>3.8809034512720002</v>
       </c>
       <c r="I199">
         <f t="shared" si="197"/>
-        <v>-1.1513285456590006</v>
+        <v>-1.4720821166699998</v>
       </c>
       <c r="J199">
         <v>1.7309167682715003</v>
@@ -9365,12 +9367,12 @@
         <v>-1.2111995332470002</v>
       </c>
       <c r="H200">
-        <f t="shared" ref="H200:I200" si="198">AVERAGE(B200:B219)</f>
-        <v>3.1421816817015</v>
+        <f t="shared" ref="H200:I200" si="198">AVERAGE(B200:B209)</f>
+        <v>3.7464516040209999</v>
       </c>
       <c r="I200">
         <f t="shared" si="198"/>
-        <v>-1.2111995332470002</v>
+        <v>-1.0579541305610001</v>
       </c>
       <c r="J200">
         <v>1.9136757402140003</v>

</xml_diff>